<commit_message>
Auto commit on 02-2025-time
</commit_message>
<xml_diff>
--- a/IM/202507_HL_Maintain_Report.xlsx
+++ b/IM/202507_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$3</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$7</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="62">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202507   (  製表日期:2025-07-01  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="96">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202507   (  製表日期:2025-07-02  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -216,6 +216,112 @@
   </si>
   <si>
     <t>O</t>
+  </si>
+  <si>
+    <t>E3853114070101</t>
+  </si>
+  <si>
+    <t>板橋互助店</t>
+  </si>
+  <si>
+    <t>新北市板橋區</t>
+  </si>
+  <si>
+    <t>2025-07-01 14:20:46</t>
+  </si>
+  <si>
+    <t>星期二</t>
+  </si>
+  <si>
+    <t>下午</t>
+  </si>
+  <si>
+    <t>HLF2</t>
+  </si>
+  <si>
+    <t>HL-CCD掃描器(TM)</t>
+  </si>
+  <si>
+    <t>F201</t>
+  </si>
+  <si>
+    <t>掃描無反應或感應不良</t>
+  </si>
+  <si>
+    <t>門市告知TM1掃描槍(HC76-TR)經常感應不良且無亮燈也無逼聲，代收沒問題但這半個月越來越多商品無法刷讀，期間已嘗試執行掃槍校正仍未改善，當下不願再次執行掃槍校正，需請台芝到店協助(感應不良)</t>
+  </si>
+  <si>
+    <t>THILF03853</t>
+  </si>
+  <si>
+    <t>狄澤洋</t>
+  </si>
+  <si>
+    <t>2025-07-01 14:50:31</t>
+  </si>
+  <si>
+    <t>2025-07-02 11:27:00</t>
+  </si>
+  <si>
+    <t>2025-07-02 11:55:00</t>
+  </si>
+  <si>
+    <t>2025-07-02 18:50:00</t>
+  </si>
+  <si>
+    <t>更換掃槍
+換上：8119012859
+換下：8119012234</t>
+  </si>
+  <si>
+    <t>E3853114070102</t>
+  </si>
+  <si>
+    <t>2025-07-01 14:22:07</t>
+  </si>
+  <si>
+    <t>門市告知TM2掃描槍(HC76-TR)經常感應不良且無亮燈也無逼聲，代收沒問題但這半個月越來越多商品無法刷讀，期間已嘗試執行掃槍校正仍未改善，當下不願再次執行掃槍校正，需請台芝到店協助(感應不良)</t>
+  </si>
+  <si>
+    <t>2025-07-01 14:52:18</t>
+  </si>
+  <si>
+    <t>2025-07-02 11:28:00</t>
+  </si>
+  <si>
+    <t>2025-07-02 18:52:00</t>
+  </si>
+  <si>
+    <t>更換掃槍
+換上：8119012486
+換下：8119012233</t>
+  </si>
+  <si>
+    <t>服務</t>
+  </si>
+  <si>
+    <t>三重永福店</t>
+  </si>
+  <si>
+    <t>THILF02349</t>
+  </si>
+  <si>
+    <t>2025-07-02 11:54:22</t>
+  </si>
+  <si>
+    <t>2025-07-02 10:40:00</t>
+  </si>
+  <si>
+    <t>2025-07-02 11:52:00</t>
+  </si>
+  <si>
+    <t>PMQ3+TVV+STAR</t>
+  </si>
+  <si>
+    <t>2025-07-02 12:31:48</t>
+  </si>
+  <si>
+    <t>PMQ3</t>
   </si>
 </sst>
 </file>
@@ -295,7 +401,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
@@ -308,6 +414,9 @@
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
@@ -319,6 +428,12 @@
     </xf>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -620,10 +735,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK3"/>
+  <dimension ref="A1:AK7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -685,7 +800,7 @@
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
-      <c r="P1" s="5"/>
+      <c r="P1" s="6"/>
       <c r="Q1" s="3"/>
       <c r="R1" s="3"/>
       <c r="S1" s="3"/>
@@ -698,7 +813,7 @@
       <c r="Z1" s="3"/>
       <c r="AA1" s="3"/>
       <c r="AB1" s="3"/>
-      <c r="AC1" s="5"/>
+      <c r="AC1" s="6"/>
       <c r="AD1" s="3"/>
       <c r="AE1" s="3"/>
       <c r="AF1" s="3"/>
@@ -822,99 +937,449 @@
       </c>
     </row>
     <row r="3" spans="1:37">
-      <c r="A3" s="6">
+      <c r="A3" s="7">
         <v>1</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="7">
         <v>2025063744</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="7">
         <v>4260</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="M3" s="7" t="s">
+      <c r="M3" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="N3" s="6" t="s">
+      <c r="N3" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="O3" s="7" t="s">
+      <c r="O3" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="P3" s="7" t="s">
+      <c r="P3" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="Q3" s="6" t="s">
+      <c r="Q3" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="R3" s="6" t="s">
+      <c r="R3" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="S3" s="6" t="s">
+      <c r="S3" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="T3" s="6">
+      <c r="T3" s="7">
         <v>1</v>
       </c>
-      <c r="U3" s="6" t="s">
+      <c r="U3" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="V3" s="6" t="s">
+      <c r="V3" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="W3" s="6" t="s">
+      <c r="W3" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="X3" s="6" t="s">
+      <c r="X3" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="Y3" s="6" t="s">
+      <c r="Y3" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="Z3" s="6">
+      <c r="Z3" s="7">
         <v>1</v>
       </c>
-      <c r="AA3" s="6"/>
-      <c r="AB3" s="6" t="s">
+      <c r="AA3" s="7"/>
+      <c r="AB3" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="AC3" s="7" t="s">
+      <c r="AC3" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="AD3" s="6"/>
-      <c r="AE3" s="6"/>
-      <c r="AF3" s="6"/>
-      <c r="AG3" s="6"/>
-      <c r="AH3" s="6"/>
-      <c r="AI3" s="6"/>
-      <c r="AJ3" s="6"/>
-      <c r="AK3" s="6" t="s">
+      <c r="AD3" s="7"/>
+      <c r="AE3" s="7"/>
+      <c r="AF3" s="7"/>
+      <c r="AG3" s="7"/>
+      <c r="AH3" s="7"/>
+      <c r="AI3" s="7"/>
+      <c r="AJ3" s="7"/>
+      <c r="AK3" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:37">
+      <c r="A4" s="3">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="3">
+        <v>2025070084</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="3">
+        <v>3853</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="P4" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="T4" s="3">
+        <v>1</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="W4" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="X4" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y4" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z4" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC4" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD4" s="3"/>
+      <c r="AE4" s="3"/>
+      <c r="AF4" s="3"/>
+      <c r="AG4" s="3"/>
+      <c r="AH4" s="3"/>
+      <c r="AI4" s="3"/>
+      <c r="AJ4" s="3"/>
+      <c r="AK4" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:37">
+      <c r="A5" s="7">
+        <v>3</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="7">
+        <v>2025070085</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="7">
+        <v>3853</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="M5" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="N5" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="O5" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="P5" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q5" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="R5" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S5" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="T5" s="7">
+        <v>1</v>
+      </c>
+      <c r="U5" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V5" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="W5" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="X5" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y5" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z5" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA5" s="7"/>
+      <c r="AB5" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC5" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="AD5" s="7"/>
+      <c r="AE5" s="7"/>
+      <c r="AF5" s="7"/>
+      <c r="AG5" s="7"/>
+      <c r="AH5" s="7"/>
+      <c r="AI5" s="7"/>
+      <c r="AJ5" s="7"/>
+      <c r="AK5" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:37">
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" s="3">
+        <v>2025070356</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3">
+        <v>2349</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S6" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T6" s="3">
+        <v>1</v>
+      </c>
+      <c r="U6" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V6" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="W6" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="X6" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="AA6" s="3"/>
+      <c r="AB6" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC6" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="AD6" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE6" s="3"/>
+      <c r="AF6" s="3"/>
+      <c r="AG6" s="3"/>
+      <c r="AH6" s="3"/>
+      <c r="AI6" s="3"/>
+      <c r="AJ6" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK6" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:37">
+      <c r="A7" s="7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" s="7">
+        <v>2025070364</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7">
+        <v>3853</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="8"/>
+      <c r="Q7" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="R7" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S7" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="T7" s="7">
+        <v>1</v>
+      </c>
+      <c r="U7" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V7" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="W7" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="X7" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y7" s="7"/>
+      <c r="Z7" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA7" s="7"/>
+      <c r="AB7" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC7" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="AD7" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE7" s="7"/>
+      <c r="AF7" s="7"/>
+      <c r="AG7" s="7"/>
+      <c r="AH7" s="7"/>
+      <c r="AI7" s="7"/>
+      <c r="AJ7" s="7"/>
+      <c r="AK7" s="7" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit on 03-2025-time
</commit_message>
<xml_diff>
--- a/IM/202507_HL_Maintain_Report.xlsx
+++ b/IM/202507_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$12</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$14</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="119">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202507   (  製表日期:2025-07-02  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="133">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202507   (  製表日期:2025-07-03  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -342,6 +342,35 @@
     <t>PMQ3+STAR</t>
   </si>
   <si>
+    <t>14196114070201</t>
+  </si>
+  <si>
+    <t>2025-07-02 13:10:24</t>
+  </si>
+  <si>
+    <t>星期三</t>
+  </si>
+  <si>
+    <t>TM2-CCD掃描器(HC56II-TR)-門市反應近期於TM2操作菸品交易，點選提醒視窗是後，再次刷讀商品會無反應，都需在面板多點幾次再刷讀才有反應，已嘗試執行TM2觸控校正、TM2-CCD掃描器校正仍無改善，且發現不只菸品，大部分的商品條碼都感應不靈敏..請台芝到店協助</t>
+  </si>
+  <si>
+    <t>2025-07-02 13:12:10</t>
+  </si>
+  <si>
+    <t>2025-07-03 11:00:00</t>
+  </si>
+  <si>
+    <t>2025-07-03 11:36:00</t>
+  </si>
+  <si>
+    <t>2025-07-03 17:12:00</t>
+  </si>
+  <si>
+    <t>更換掃描槍
+換下8119008740
+換上8119012487</t>
+  </si>
+  <si>
     <t>三重溪美店</t>
   </si>
   <si>
@@ -391,6 +420,21 @@
   </si>
   <si>
     <t>2025-07-02 17:13:00</t>
+  </si>
+  <si>
+    <t>三重公園店</t>
+  </si>
+  <si>
+    <t>THILF04352</t>
+  </si>
+  <si>
+    <t>2025-07-03 12:49:15</t>
+  </si>
+  <si>
+    <t>2025-07-03 12:00:00</t>
+  </si>
+  <si>
+    <t>2025-07-03 12:48:00</t>
   </si>
 </sst>
 </file>
@@ -804,10 +848,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK12"/>
+  <dimension ref="A1:AK14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="AC9" sqref="AC9"/>
+      <selection activeCell="AC11" sqref="AC11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1536,32 +1580,52 @@
         <v>7</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>87</v>
+        <v>38</v>
       </c>
       <c r="C9" s="7">
-        <v>2025070395</v>
-      </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
+        <v>2025070370</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="F9" s="7">
-        <v>4191</v>
+        <v>4196</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="H9" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="9"/>
+      <c r="I9" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="L9" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="M9" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="N9" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="O9" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="P9" s="9" t="s">
+        <v>105</v>
+      </c>
       <c r="Q9" s="7" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="R9" s="7" t="s">
         <v>52</v>
@@ -1576,36 +1640,34 @@
         <v>54</v>
       </c>
       <c r="V9" s="7" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="W9" s="7" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="X9" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="Y9" s="7"/>
+        <v>108</v>
+      </c>
+      <c r="Y9" s="7" t="s">
+        <v>109</v>
+      </c>
       <c r="Z9" s="7">
-        <v>1.1</v>
+        <v>0.6</v>
       </c>
       <c r="AA9" s="7"/>
       <c r="AB9" s="7" t="s">
         <v>59</v>
       </c>
       <c r="AC9" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="AD9" s="7" t="s">
-        <v>61</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="AD9" s="7"/>
       <c r="AE9" s="7"/>
       <c r="AF9" s="7"/>
       <c r="AG9" s="7"/>
       <c r="AH9" s="7"/>
       <c r="AI9" s="7"/>
-      <c r="AJ9" s="7" t="s">
-        <v>61</v>
-      </c>
+      <c r="AJ9" s="7"/>
       <c r="AK9" s="7" t="s">
         <v>61</v>
       </c>
@@ -1618,15 +1680,15 @@
         <v>87</v>
       </c>
       <c r="C10" s="3">
-        <v>2025070417</v>
+        <v>2025070395</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3">
-        <v>4210</v>
+        <v>4191</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>42</v>
@@ -1640,7 +1702,7 @@
       <c r="O10" s="4"/>
       <c r="P10" s="10"/>
       <c r="Q10" s="3" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="R10" s="3" t="s">
         <v>52</v>
@@ -1655,24 +1717,24 @@
         <v>54</v>
       </c>
       <c r="V10" s="3" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="W10" s="3" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="X10" s="3" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="Y10" s="3"/>
       <c r="Z10" s="3">
-        <v>1</v>
+        <v>1.1</v>
       </c>
       <c r="AA10" s="3"/>
       <c r="AB10" s="3" t="s">
         <v>59</v>
       </c>
       <c r="AC10" s="10" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="AD10" s="3" t="s">
         <v>61</v>
@@ -1697,7 +1759,7 @@
         <v>87</v>
       </c>
       <c r="C11" s="7">
-        <v>2025070428</v>
+        <v>2025070417</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
@@ -1705,7 +1767,7 @@
         <v>4210</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="H11" s="7" t="s">
         <v>42</v>
@@ -1719,7 +1781,7 @@
       <c r="O11" s="8"/>
       <c r="P11" s="9"/>
       <c r="Q11" s="7" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="R11" s="7" t="s">
         <v>52</v>
@@ -1734,13 +1796,13 @@
         <v>54</v>
       </c>
       <c r="V11" s="7" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="W11" s="7" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="X11" s="7" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="Y11" s="7"/>
       <c r="Z11" s="7">
@@ -1776,15 +1838,15 @@
         <v>87</v>
       </c>
       <c r="C12" s="3">
-        <v>2025070429</v>
+        <v>2025070428</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
-      <c r="F12" s="3" t="s">
-        <v>113</v>
+      <c r="F12" s="3">
+        <v>4210</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>42</v>
@@ -1796,9 +1858,9 @@
       <c r="M12" s="4"/>
       <c r="N12" s="3"/>
       <c r="O12" s="4"/>
-      <c r="P12" s="4"/>
+      <c r="P12" s="10"/>
       <c r="Q12" s="3" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="R12" s="3" t="s">
         <v>52</v>
@@ -1813,23 +1875,23 @@
         <v>54</v>
       </c>
       <c r="V12" s="3" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="W12" s="3" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="X12" s="3" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="Y12" s="3"/>
       <c r="Z12" s="3">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="AA12" s="3"/>
       <c r="AB12" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="AC12" s="4" t="s">
+      <c r="AC12" s="10" t="s">
         <v>101</v>
       </c>
       <c r="AD12" s="3" t="s">
@@ -1844,6 +1906,164 @@
         <v>61</v>
       </c>
       <c r="AK12" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:37">
+      <c r="A13" s="7">
+        <v>11</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C13" s="7">
+        <v>2025070429</v>
+      </c>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="R13" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S13" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="T13" s="7">
+        <v>1</v>
+      </c>
+      <c r="U13" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V13" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="W13" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="X13" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="Y13" s="7"/>
+      <c r="Z13" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="AA13" s="7"/>
+      <c r="AB13" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC13" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="AD13" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE13" s="7"/>
+      <c r="AF13" s="7"/>
+      <c r="AG13" s="7"/>
+      <c r="AH13" s="7"/>
+      <c r="AI13" s="7"/>
+      <c r="AJ13" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK13" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:37">
+      <c r="A14" s="3">
+        <v>12</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C14" s="3">
+        <v>2025070534</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3">
+        <v>4352</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="R14" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S14" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T14" s="3">
+        <v>1</v>
+      </c>
+      <c r="U14" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V14" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="W14" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="X14" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y14" s="3"/>
+      <c r="Z14" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="AA14" s="3"/>
+      <c r="AB14" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC14" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="AD14" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE14" s="3"/>
+      <c r="AF14" s="3"/>
+      <c r="AG14" s="3"/>
+      <c r="AH14" s="3"/>
+      <c r="AI14" s="3"/>
+      <c r="AJ14" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK14" s="3" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit on 04-2025-time
</commit_message>
<xml_diff>
--- a/IM/202507_HL_Maintain_Report.xlsx
+++ b/IM/202507_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$14</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$28</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="133">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202507   (  製表日期:2025-07-03  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="219">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202507   (  製表日期:2025-07-04  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -435,6 +435,266 @@
   </si>
   <si>
     <t>2025-07-03 12:48:00</t>
+  </si>
+  <si>
+    <t>新莊雙鳳店</t>
+  </si>
+  <si>
+    <t>新北市新莊區</t>
+  </si>
+  <si>
+    <t>THILF04005</t>
+  </si>
+  <si>
+    <t>湯家瑋</t>
+  </si>
+  <si>
+    <t>2025-07-03 13:26:40</t>
+  </si>
+  <si>
+    <t>2025-07-03 13:00:00</t>
+  </si>
+  <si>
+    <t>2025-07-03 13:20:00</t>
+  </si>
+  <si>
+    <t>D174</t>
+  </si>
+  <si>
+    <t>新莊裕民店</t>
+  </si>
+  <si>
+    <t>THILF0D174</t>
+  </si>
+  <si>
+    <t>2025-07-03 13:40:10</t>
+  </si>
+  <si>
+    <t>2025-07-03 13:40:00</t>
+  </si>
+  <si>
+    <t>三重大院店</t>
+  </si>
+  <si>
+    <t>THILF04560</t>
+  </si>
+  <si>
+    <t>2025-07-03 13:43:57</t>
+  </si>
+  <si>
+    <t>2025-07-03 13:43:00</t>
+  </si>
+  <si>
+    <t>D148</t>
+  </si>
+  <si>
+    <t>新莊福營店</t>
+  </si>
+  <si>
+    <t>THILF0D148</t>
+  </si>
+  <si>
+    <t>2025-07-03 13:57:19</t>
+  </si>
+  <si>
+    <t>2025-07-03 14:00:00</t>
+  </si>
+  <si>
+    <t>L562</t>
+  </si>
+  <si>
+    <t>田倉民安店</t>
+  </si>
+  <si>
+    <t>THILF0L562</t>
+  </si>
+  <si>
+    <t>2025-07-03 14:15:18</t>
+  </si>
+  <si>
+    <t>2025-07-03 14:15:00</t>
+  </si>
+  <si>
+    <t>三重三和夜市</t>
+  </si>
+  <si>
+    <t>THILF02303</t>
+  </si>
+  <si>
+    <t>2025-07-03 14:59:00</t>
+  </si>
+  <si>
+    <t>2025-07-03 14:58:00</t>
+  </si>
+  <si>
+    <t>12303114070301</t>
+  </si>
+  <si>
+    <t>2025-07-03 15:31:29</t>
+  </si>
+  <si>
+    <t>星期四</t>
+  </si>
+  <si>
+    <t>HL23</t>
+  </si>
+  <si>
+    <t>HL-TM主機</t>
+  </si>
+  <si>
+    <t>抽屜無法正常開關</t>
+  </si>
+  <si>
+    <t>門市反應TM2(TCX800)抽屜的鎖頭不見，抽屜外觀白/鑰匙孔位置中間/沒有鎖頭...需請台芝到店協助</t>
+  </si>
+  <si>
+    <t>2025-07-03 15:38:29</t>
+  </si>
+  <si>
+    <t>2025-07-04 13:03:00</t>
+  </si>
+  <si>
+    <t>2025-07-04 13:33:00</t>
+  </si>
+  <si>
+    <t>2025-07-04 19:38:00</t>
+  </si>
+  <si>
+    <t>更換錢箱
+換下81Z1000818
+換上81Z1004345</t>
+  </si>
+  <si>
+    <t>三重中央北店</t>
+  </si>
+  <si>
+    <t>THILF02042</t>
+  </si>
+  <si>
+    <t>2025-07-03 16:07:54</t>
+  </si>
+  <si>
+    <t>2025-07-03 15:10:00</t>
+  </si>
+  <si>
+    <t>2025-07-03 16:07:00</t>
+  </si>
+  <si>
+    <t>三重龍濱店</t>
+  </si>
+  <si>
+    <t>THILF04029</t>
+  </si>
+  <si>
+    <t>2025-07-03 17:27:19</t>
+  </si>
+  <si>
+    <t>2025-07-03 16:10:00</t>
+  </si>
+  <si>
+    <t>2025-07-03 17:01:00</t>
+  </si>
+  <si>
+    <t>E2301114070401</t>
+  </si>
+  <si>
+    <t>蘆洲樂平店</t>
+  </si>
+  <si>
+    <t>新北市蘆洲區</t>
+  </si>
+  <si>
+    <t>2025-07-04 07:00:19</t>
+  </si>
+  <si>
+    <t>星期五</t>
+  </si>
+  <si>
+    <t>凌晨</t>
+  </si>
+  <si>
+    <t>HL58</t>
+  </si>
+  <si>
+    <t>HL-LIFE-ET主機</t>
+  </si>
+  <si>
+    <t>無法連線</t>
+  </si>
+  <si>
+    <t>門市反應MMK四代機無法連線，重啟後畫面出現網路設定介面視窗但照步驟操作重開機後也異常，ping60不通....須請台芝到店協助(半夜跳電後就無法連上網路)</t>
+  </si>
+  <si>
+    <t>THILF02301</t>
+  </si>
+  <si>
+    <t>2025-07-04 09:04:13</t>
+  </si>
+  <si>
+    <t>2025-07-04 11:00:00</t>
+  </si>
+  <si>
+    <t>2025-07-04 12:09:00</t>
+  </si>
+  <si>
+    <t>2025-07-07 13:04:00</t>
+  </si>
+  <si>
+    <t>重新啟動，設定及連線皆為正常</t>
+  </si>
+  <si>
+    <t>泰山新民店</t>
+  </si>
+  <si>
+    <t>新北市泰山區</t>
+  </si>
+  <si>
+    <t>THILF04656</t>
+  </si>
+  <si>
+    <t>2025-07-04 10:49:24</t>
+  </si>
+  <si>
+    <t>2025-07-04 10:30:00</t>
+  </si>
+  <si>
+    <t>2025-07-04 10:50:00</t>
+  </si>
+  <si>
+    <t>北縣泰富店</t>
+  </si>
+  <si>
+    <t>THILF03606</t>
+  </si>
+  <si>
+    <t>2025-07-04 11:27:27</t>
+  </si>
+  <si>
+    <t>2025-07-04 10:55:00</t>
+  </si>
+  <si>
+    <t>2025-07-04 11:20:00</t>
+  </si>
+  <si>
+    <t>2025-07-04 12:13:16</t>
+  </si>
+  <si>
+    <t>2025-07-04 12:12:00</t>
+  </si>
+  <si>
+    <t>蘆洲永樂店</t>
+  </si>
+  <si>
+    <t>THILF04036</t>
+  </si>
+  <si>
+    <t>2025-07-04 12:45:17</t>
+  </si>
+  <si>
+    <t>2025-07-04 12:10:00</t>
+  </si>
+  <si>
+    <t>2025-07-04 12:44:00</t>
   </si>
 </sst>
 </file>
@@ -848,10 +1108,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK14"/>
+  <dimension ref="A1:AK28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="AC11" sqref="AC11"/>
+      <selection activeCell="AC25" sqref="AC25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2016,7 +2276,7 @@
       <c r="M14" s="4"/>
       <c r="N14" s="3"/>
       <c r="O14" s="4"/>
-      <c r="P14" s="4"/>
+      <c r="P14" s="10"/>
       <c r="Q14" s="3" t="s">
         <v>129</v>
       </c>
@@ -2049,7 +2309,7 @@
       <c r="AB14" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="AC14" s="4" t="s">
+      <c r="AC14" s="10" t="s">
         <v>101</v>
       </c>
       <c r="AD14" s="3" t="s">
@@ -2064,6 +2324,1134 @@
         <v>61</v>
       </c>
       <c r="AK14" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:37">
+      <c r="A15" s="7">
+        <v>13</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C15" s="7">
+        <v>2025070545</v>
+      </c>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7">
+        <v>4005</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="R15" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S15" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="T15" s="7">
+        <v>1</v>
+      </c>
+      <c r="U15" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V15" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="W15" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="X15" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="Y15" s="7"/>
+      <c r="Z15" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA15" s="7"/>
+      <c r="AB15" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC15" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="AD15" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE15" s="7"/>
+      <c r="AF15" s="7"/>
+      <c r="AG15" s="7"/>
+      <c r="AH15" s="7"/>
+      <c r="AI15" s="7"/>
+      <c r="AJ15" s="7"/>
+      <c r="AK15" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:37">
+      <c r="A16" s="3">
+        <v>14</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C16" s="3">
+        <v>2025070547</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="10"/>
+      <c r="Q16" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="R16" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S16" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="T16" s="3">
+        <v>1</v>
+      </c>
+      <c r="U16" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V16" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="W16" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="X16" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="Y16" s="3"/>
+      <c r="Z16" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA16" s="3"/>
+      <c r="AB16" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC16" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="AD16" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE16" s="3"/>
+      <c r="AF16" s="3"/>
+      <c r="AG16" s="3"/>
+      <c r="AH16" s="3"/>
+      <c r="AI16" s="3"/>
+      <c r="AJ16" s="3"/>
+      <c r="AK16" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:37">
+      <c r="A17" s="7">
+        <v>15</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C17" s="7">
+        <v>2025070548</v>
+      </c>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7">
+        <v>4560</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="7"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="R17" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S17" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="T17" s="7">
+        <v>1</v>
+      </c>
+      <c r="U17" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V17" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="W17" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="X17" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="Y17" s="7"/>
+      <c r="Z17" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="AA17" s="7"/>
+      <c r="AB17" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC17" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="AD17" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE17" s="7"/>
+      <c r="AF17" s="7"/>
+      <c r="AG17" s="7"/>
+      <c r="AH17" s="7"/>
+      <c r="AI17" s="7"/>
+      <c r="AJ17" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK17" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:37">
+      <c r="A18" s="3">
+        <v>16</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C18" s="3">
+        <v>2025070551</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="10"/>
+      <c r="Q18" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="R18" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S18" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="T18" s="3">
+        <v>1</v>
+      </c>
+      <c r="U18" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V18" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="W18" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="X18" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="Y18" s="3"/>
+      <c r="Z18" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA18" s="3"/>
+      <c r="AB18" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC18" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="AD18" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE18" s="3"/>
+      <c r="AF18" s="3"/>
+      <c r="AG18" s="3"/>
+      <c r="AH18" s="3"/>
+      <c r="AI18" s="3"/>
+      <c r="AJ18" s="3"/>
+      <c r="AK18" s="3"/>
+    </row>
+    <row r="19" spans="1:37">
+      <c r="A19" s="7">
+        <v>17</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C19" s="7">
+        <v>2025070557</v>
+      </c>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="R19" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S19" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="T19" s="7">
+        <v>1</v>
+      </c>
+      <c r="U19" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V19" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="W19" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="X19" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="Y19" s="7"/>
+      <c r="Z19" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA19" s="7"/>
+      <c r="AB19" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC19" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="AD19" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE19" s="7"/>
+      <c r="AF19" s="7"/>
+      <c r="AG19" s="7"/>
+      <c r="AH19" s="7"/>
+      <c r="AI19" s="7"/>
+      <c r="AJ19" s="7"/>
+      <c r="AK19" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:37">
+      <c r="A20" s="3">
+        <v>18</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C20" s="3">
+        <v>2025070565</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3">
+        <v>2303</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="10"/>
+      <c r="Q20" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="R20" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S20" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T20" s="3">
+        <v>1</v>
+      </c>
+      <c r="U20" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V20" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="W20" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="X20" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="Y20" s="3"/>
+      <c r="Z20" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA20" s="3"/>
+      <c r="AB20" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC20" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="AD20" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE20" s="3"/>
+      <c r="AF20" s="3"/>
+      <c r="AG20" s="3"/>
+      <c r="AH20" s="3"/>
+      <c r="AI20" s="3"/>
+      <c r="AJ20" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK20" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:37">
+      <c r="A21" s="7">
+        <v>19</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="7">
+        <v>2025070577</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F21" s="7">
+        <v>2303</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="J21" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="K21" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="L21" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="M21" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="N21" s="7">
+        <v>2305</v>
+      </c>
+      <c r="O21" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="P21" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="Q21" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="R21" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S21" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="T21" s="7">
+        <v>1</v>
+      </c>
+      <c r="U21" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V21" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="W21" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="X21" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="Y21" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="Z21" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA21" s="7"/>
+      <c r="AB21" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC21" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="AD21" s="7"/>
+      <c r="AE21" s="7"/>
+      <c r="AF21" s="7"/>
+      <c r="AG21" s="7"/>
+      <c r="AH21" s="7"/>
+      <c r="AI21" s="7"/>
+      <c r="AJ21" s="7"/>
+      <c r="AK21" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:37">
+      <c r="A22" s="3">
+        <v>20</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C22" s="3">
+        <v>2025070586</v>
+      </c>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3">
+        <v>2042</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="4"/>
+      <c r="P22" s="10"/>
+      <c r="Q22" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="R22" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S22" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T22" s="3">
+        <v>1</v>
+      </c>
+      <c r="U22" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V22" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="W22" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="X22" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="Y22" s="3"/>
+      <c r="Z22" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA22" s="3"/>
+      <c r="AB22" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC22" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="AD22" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE22" s="3"/>
+      <c r="AF22" s="3"/>
+      <c r="AG22" s="3"/>
+      <c r="AH22" s="3"/>
+      <c r="AI22" s="3"/>
+      <c r="AJ22" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK22" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:37">
+      <c r="A23" s="7">
+        <v>21</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C23" s="7">
+        <v>2025070602</v>
+      </c>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7">
+        <v>4029</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="8"/>
+      <c r="N23" s="7"/>
+      <c r="O23" s="8"/>
+      <c r="P23" s="9"/>
+      <c r="Q23" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="R23" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S23" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="T23" s="7">
+        <v>1</v>
+      </c>
+      <c r="U23" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V23" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="W23" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="X23" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="Y23" s="7"/>
+      <c r="Z23" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="AA23" s="7"/>
+      <c r="AB23" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC23" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="AD23" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE23" s="7"/>
+      <c r="AF23" s="7"/>
+      <c r="AG23" s="7"/>
+      <c r="AH23" s="7"/>
+      <c r="AI23" s="7"/>
+      <c r="AJ23" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK23" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:37">
+      <c r="A24" s="3">
+        <v>22</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="3">
+        <v>2025070632</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F24" s="3">
+        <v>2301</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="M24" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="N24" s="3">
+        <v>5804</v>
+      </c>
+      <c r="O24" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="P24" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="Q24" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="R24" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S24" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T24" s="3">
+        <v>1</v>
+      </c>
+      <c r="U24" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V24" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="W24" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="X24" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="Y24" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="Z24" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="AA24" s="3"/>
+      <c r="AB24" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC24" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="AD24" s="3"/>
+      <c r="AE24" s="3"/>
+      <c r="AF24" s="3"/>
+      <c r="AG24" s="3"/>
+      <c r="AH24" s="3"/>
+      <c r="AI24" s="3"/>
+      <c r="AJ24" s="3"/>
+      <c r="AK24" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:37">
+      <c r="A25" s="7">
+        <v>23</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C25" s="7">
+        <v>2025070689</v>
+      </c>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7">
+        <v>4656</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="8"/>
+      <c r="N25" s="7"/>
+      <c r="O25" s="8"/>
+      <c r="P25" s="9"/>
+      <c r="Q25" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="R25" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S25" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="T25" s="7">
+        <v>1</v>
+      </c>
+      <c r="U25" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V25" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="W25" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="X25" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="Y25" s="7"/>
+      <c r="Z25" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA25" s="7"/>
+      <c r="AB25" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC25" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="AD25" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE25" s="7"/>
+      <c r="AF25" s="7"/>
+      <c r="AG25" s="7"/>
+      <c r="AH25" s="7"/>
+      <c r="AI25" s="7"/>
+      <c r="AJ25" s="7"/>
+      <c r="AK25" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="1:37">
+      <c r="A26" s="3">
+        <v>24</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C26" s="3">
+        <v>2025070706</v>
+      </c>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3">
+        <v>3606</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="4"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="4"/>
+      <c r="P26" s="10"/>
+      <c r="Q26" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="R26" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S26" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="T26" s="3">
+        <v>1</v>
+      </c>
+      <c r="U26" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V26" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="W26" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="X26" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="Y26" s="3"/>
+      <c r="Z26" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="AA26" s="3"/>
+      <c r="AB26" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC26" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="AD26" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE26" s="3"/>
+      <c r="AF26" s="3"/>
+      <c r="AG26" s="3"/>
+      <c r="AH26" s="3"/>
+      <c r="AI26" s="3"/>
+      <c r="AJ26" s="3"/>
+      <c r="AK26" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:37">
+      <c r="A27" s="7">
+        <v>25</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C27" s="7">
+        <v>2025070719</v>
+      </c>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7">
+        <v>2301</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="H27" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="7"/>
+      <c r="L27" s="7"/>
+      <c r="M27" s="8"/>
+      <c r="N27" s="7"/>
+      <c r="O27" s="8"/>
+      <c r="P27" s="9"/>
+      <c r="Q27" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="R27" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S27" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="T27" s="7">
+        <v>1</v>
+      </c>
+      <c r="U27" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V27" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="W27" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="X27" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="Y27" s="7"/>
+      <c r="Z27" s="7">
+        <v>1.2</v>
+      </c>
+      <c r="AA27" s="7"/>
+      <c r="AB27" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC27" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="AD27" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE27" s="7"/>
+      <c r="AF27" s="7"/>
+      <c r="AG27" s="7"/>
+      <c r="AH27" s="7"/>
+      <c r="AI27" s="7"/>
+      <c r="AJ27" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK27" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:37">
+      <c r="A28" s="3">
+        <v>26</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C28" s="3">
+        <v>2025070721</v>
+      </c>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3">
+        <v>4036</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="4"/>
+      <c r="N28" s="3"/>
+      <c r="O28" s="4"/>
+      <c r="P28" s="4"/>
+      <c r="Q28" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="R28" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S28" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T28" s="3">
+        <v>1</v>
+      </c>
+      <c r="U28" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V28" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="W28" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="X28" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="Y28" s="3"/>
+      <c r="Z28" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="AA28" s="3"/>
+      <c r="AB28" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC28" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="AD28" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE28" s="3"/>
+      <c r="AF28" s="3"/>
+      <c r="AG28" s="3"/>
+      <c r="AH28" s="3"/>
+      <c r="AI28" s="3"/>
+      <c r="AJ28" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK28" s="3" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit on 07-2025-time
</commit_message>
<xml_diff>
--- a/IM/202507_HL_Maintain_Report.xlsx
+++ b/IM/202507_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$31</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$34</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="235">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202507   (  製表日期:2025-07-04  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="256">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202507   (  製表日期:2025-07-07  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -743,6 +743,71 @@
   </si>
   <si>
     <t>2025-07-04 16:08:00</t>
+  </si>
+  <si>
+    <t>E2222114070501</t>
+  </si>
+  <si>
+    <t>三重義天店</t>
+  </si>
+  <si>
+    <t>2025-07-05 06:56:55</t>
+  </si>
+  <si>
+    <t>星期六</t>
+  </si>
+  <si>
+    <t>無電源反應、無法開機</t>
+  </si>
+  <si>
+    <t>門市反應tm1(TCX800)無電源反應電源未亮燈，門市已有拔插頭休息更換過插座都無法開機，ping80不通無法vnc...須請台芝到店協助(無法開機....)
+PS.若因更換HD.請跟店長宣達:1.請門市先回報代收會計 2.請確認SC的代收資料是否正確 (須與代收單據逐一核對)
+門市今日未清帳入帳日7/5不確定是否有交易</t>
+  </si>
+  <si>
+    <t>THILF02222</t>
+  </si>
+  <si>
+    <t>2025-07-05 09:13:00</t>
+  </si>
+  <si>
+    <t>2025-07-07 10:40:00</t>
+  </si>
+  <si>
+    <t>2025-07-07 11:10:00</t>
+  </si>
+  <si>
+    <t>2025-07-08 13:00:00</t>
+  </si>
+  <si>
+    <t>電源變壓器鬆脫，插回後正常</t>
+  </si>
+  <si>
+    <t>三重美堤店</t>
+  </si>
+  <si>
+    <t>THILF03890</t>
+  </si>
+  <si>
+    <t>2025-07-06 16:09:17</t>
+  </si>
+  <si>
+    <t>2025-07-06 14:30:00</t>
+  </si>
+  <si>
+    <t>2025-07-06 16:00:00</t>
+  </si>
+  <si>
+    <t>緊急撤機</t>
+  </si>
+  <si>
+    <t>2025-07-06 16:09:53</t>
+  </si>
+  <si>
+    <t>2025-07-06 16:08:00</t>
+  </si>
+  <si>
+    <t>因颱風來襲進行臨時撤店</t>
   </si>
 </sst>
 </file>
@@ -1156,10 +1221,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK31"/>
+  <dimension ref="A1:AK34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="AC31" sqref="AC31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3689,7 +3754,7 @@
       <c r="M31" s="8"/>
       <c r="N31" s="7"/>
       <c r="O31" s="8"/>
-      <c r="P31" s="8"/>
+      <c r="P31" s="9"/>
       <c r="Q31" s="7" t="s">
         <v>231</v>
       </c>
@@ -3722,7 +3787,7 @@
       <c r="AB31" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="AC31" s="8" t="s">
+      <c r="AC31" s="9" t="s">
         <v>101</v>
       </c>
       <c r="AD31" s="7" t="s">
@@ -3737,6 +3802,257 @@
         <v>61</v>
       </c>
       <c r="AK31" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:37">
+      <c r="A32" s="3">
+        <v>30</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" s="3">
+        <v>2025070890</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F32" s="3">
+        <v>2222</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="J32" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="K32" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="L32" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="M32" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="N32" s="3">
+        <v>2306</v>
+      </c>
+      <c r="O32" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="P32" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="Q32" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="R32" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S32" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T32" s="3">
+        <v>1</v>
+      </c>
+      <c r="U32" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V32" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="W32" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="X32" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y32" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="Z32" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA32" s="3"/>
+      <c r="AB32" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC32" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="AD32" s="3"/>
+      <c r="AE32" s="3"/>
+      <c r="AF32" s="3"/>
+      <c r="AG32" s="3"/>
+      <c r="AH32" s="3"/>
+      <c r="AI32" s="3"/>
+      <c r="AJ32" s="3"/>
+      <c r="AK32" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="33" spans="1:37">
+      <c r="A33" s="7">
+        <v>31</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C33" s="7">
+        <v>2025070905</v>
+      </c>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7">
+        <v>3890</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="H33" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="7"/>
+      <c r="L33" s="7"/>
+      <c r="M33" s="8"/>
+      <c r="N33" s="7"/>
+      <c r="O33" s="8"/>
+      <c r="P33" s="9"/>
+      <c r="Q33" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="R33" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S33" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="T33" s="7">
+        <v>1</v>
+      </c>
+      <c r="U33" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V33" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="W33" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="X33" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="Y33" s="7"/>
+      <c r="Z33" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="AA33" s="7"/>
+      <c r="AB33" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC33" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="AD33" s="7"/>
+      <c r="AE33" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF33" s="7"/>
+      <c r="AG33" s="7"/>
+      <c r="AH33" s="7"/>
+      <c r="AI33" s="7"/>
+      <c r="AJ33" s="7"/>
+      <c r="AK33" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" spans="1:37">
+      <c r="A34" s="3">
+        <v>32</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C34" s="3">
+        <v>2025070906</v>
+      </c>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3">
+        <v>3890</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="3"/>
+      <c r="L34" s="3"/>
+      <c r="M34" s="4"/>
+      <c r="N34" s="3"/>
+      <c r="O34" s="4"/>
+      <c r="P34" s="4"/>
+      <c r="Q34" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="R34" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S34" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T34" s="3">
+        <v>1</v>
+      </c>
+      <c r="U34" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V34" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="W34" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="X34" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="Y34" s="3"/>
+      <c r="Z34" s="3">
+        <v>1.6</v>
+      </c>
+      <c r="AA34" s="3"/>
+      <c r="AB34" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC34" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="AD34" s="3"/>
+      <c r="AE34" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF34" s="3"/>
+      <c r="AG34" s="3"/>
+      <c r="AH34" s="3"/>
+      <c r="AI34" s="3"/>
+      <c r="AJ34" s="3"/>
+      <c r="AK34" s="3" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit on 08-2025-time
</commit_message>
<xml_diff>
--- a/IM/202507_HL_Maintain_Report.xlsx
+++ b/IM/202507_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$35</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$37</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="260">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202507   (  製表日期:2025-07-07  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="275">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202507   (  製表日期:2025-07-08  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -810,6 +810,42 @@
     <t>因颱風來襲進行臨時撤店</t>
   </si>
   <si>
+    <t>15080114070701</t>
+  </si>
+  <si>
+    <t>三芝楓愛林</t>
+  </si>
+  <si>
+    <t>新北市三芝區</t>
+  </si>
+  <si>
+    <t>2025-07-07 09:39:22</t>
+  </si>
+  <si>
+    <t>上午</t>
+  </si>
+  <si>
+    <t>門市反應mmk4代機無連線畫面顯示尚未連接到網路，門市已重開多次畫面無跳出設定介面視窗，重新拔插7port仍異常，ping60不通....須請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF05080</t>
+  </si>
+  <si>
+    <t>2025-07-07 09:41:20</t>
+  </si>
+  <si>
+    <t>2025-07-08 11:27:00</t>
+  </si>
+  <si>
+    <t>2025-07-08 11:57:00</t>
+  </si>
+  <si>
+    <t>2025-07-08 13:41:00</t>
+  </si>
+  <si>
+    <t>重啟後重新設定，偵測網路皆為正常</t>
+  </si>
+  <si>
     <t>2025-07-07 17:31:46</t>
   </si>
   <si>
@@ -820,6 +856,15 @@
   </si>
   <si>
     <t>重新回裝已完工</t>
+  </si>
+  <si>
+    <t>2025-07-08 12:00:14</t>
+  </si>
+  <si>
+    <t>2025-07-08 11:30:00</t>
+  </si>
+  <si>
+    <t>2025-07-08 11:59:00</t>
   </si>
 </sst>
 </file>
@@ -1233,10 +1278,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK35"/>
+  <dimension ref="A1:AK37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A35" sqref="A35"/>
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4073,32 +4118,52 @@
         <v>33</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>87</v>
+        <v>38</v>
       </c>
       <c r="C35" s="7">
-        <v>2025071115</v>
-      </c>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
+        <v>2025070917</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="F35" s="7">
-        <v>3890</v>
+        <v>5080</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>247</v>
+        <v>257</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="I35" s="7"/>
-      <c r="J35" s="7"/>
-      <c r="K35" s="7"/>
-      <c r="L35" s="7"/>
-      <c r="M35" s="8"/>
-      <c r="N35" s="7"/>
-      <c r="O35" s="8"/>
-      <c r="P35" s="8"/>
+        <v>258</v>
+      </c>
+      <c r="I35" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="J35" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="K35" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="L35" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="M35" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="N35" s="7">
+        <v>5804</v>
+      </c>
+      <c r="O35" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="P35" s="9" t="s">
+        <v>261</v>
+      </c>
       <c r="Q35" s="7" t="s">
-        <v>248</v>
+        <v>262</v>
       </c>
       <c r="R35" s="7" t="s">
         <v>52</v>
@@ -4113,35 +4178,189 @@
         <v>54</v>
       </c>
       <c r="V35" s="7" t="s">
-        <v>256</v>
+        <v>263</v>
       </c>
       <c r="W35" s="7" t="s">
-        <v>257</v>
+        <v>264</v>
       </c>
       <c r="X35" s="7" t="s">
-        <v>258</v>
-      </c>
-      <c r="Y35" s="7"/>
+        <v>265</v>
+      </c>
+      <c r="Y35" s="7" t="s">
+        <v>266</v>
+      </c>
       <c r="Z35" s="7">
-        <v>3.5</v>
+        <v>0.5</v>
       </c>
       <c r="AA35" s="7"/>
       <c r="AB35" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="AC35" s="8" t="s">
-        <v>259</v>
+      <c r="AC35" s="9" t="s">
+        <v>267</v>
       </c>
       <c r="AD35" s="7"/>
-      <c r="AE35" s="7" t="s">
-        <v>61</v>
-      </c>
+      <c r="AE35" s="7"/>
       <c r="AF35" s="7"/>
       <c r="AG35" s="7"/>
       <c r="AH35" s="7"/>
       <c r="AI35" s="7"/>
       <c r="AJ35" s="7"/>
       <c r="AK35" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36" spans="1:37">
+      <c r="A36" s="3">
+        <v>34</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C36" s="3">
+        <v>2025071115</v>
+      </c>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3">
+        <v>3890</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+      <c r="L36" s="3"/>
+      <c r="M36" s="4"/>
+      <c r="N36" s="3"/>
+      <c r="O36" s="4"/>
+      <c r="P36" s="10"/>
+      <c r="Q36" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="R36" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S36" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T36" s="3">
+        <v>1</v>
+      </c>
+      <c r="U36" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V36" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="W36" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="X36" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="Y36" s="3"/>
+      <c r="Z36" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="AA36" s="3"/>
+      <c r="AB36" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC36" s="10" t="s">
+        <v>271</v>
+      </c>
+      <c r="AD36" s="3"/>
+      <c r="AE36" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF36" s="3"/>
+      <c r="AG36" s="3"/>
+      <c r="AH36" s="3"/>
+      <c r="AI36" s="3"/>
+      <c r="AJ36" s="3"/>
+      <c r="AK36" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="37" spans="1:37">
+      <c r="A37" s="7">
+        <v>35</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C37" s="7">
+        <v>2025071149</v>
+      </c>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7">
+        <v>5080</v>
+      </c>
+      <c r="G37" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="H37" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="I37" s="7"/>
+      <c r="J37" s="7"/>
+      <c r="K37" s="7"/>
+      <c r="L37" s="7"/>
+      <c r="M37" s="8"/>
+      <c r="N37" s="7"/>
+      <c r="O37" s="8"/>
+      <c r="P37" s="8"/>
+      <c r="Q37" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="R37" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S37" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="T37" s="7">
+        <v>1</v>
+      </c>
+      <c r="U37" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V37" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="W37" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="X37" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="Y37" s="7"/>
+      <c r="Z37" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA37" s="7"/>
+      <c r="AB37" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC37" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="AD37" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE37" s="7"/>
+      <c r="AF37" s="7"/>
+      <c r="AG37" s="7"/>
+      <c r="AH37" s="7"/>
+      <c r="AI37" s="7"/>
+      <c r="AJ37" s="7"/>
+      <c r="AK37" s="7" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit on 14-2025-time
</commit_message>
<xml_diff>
--- a/IM/202507_HL_Maintain_Report.xlsx
+++ b/IM/202507_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$62</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$71</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="422">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202507   (  製表日期:2025-07-11  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="476">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202507   (  製表日期:2025-07-14  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -1312,6 +1312,170 @@
   </si>
   <si>
     <t>變壓器鬆脫，插緊後正常</t>
+  </si>
+  <si>
+    <t>14167114071101</t>
+  </si>
+  <si>
+    <t>板橋松翠店</t>
+  </si>
+  <si>
+    <t>2025-07-11 15:21:46</t>
+  </si>
+  <si>
+    <t>觸控不良(游標偏移)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">門市反應TM1(TCX800)觸控與TM2相比會較遲緩，例:咖啡快速鍵內點選咖啡商品鍵會延遲幾秒才帶入品項，客服已協助執行觸控校正後仍異常...請台芝到店協助
+</t>
+  </si>
+  <si>
+    <t>THILF04167</t>
+  </si>
+  <si>
+    <t>2025-07-11 15:30:57</t>
+  </si>
+  <si>
+    <t>2025-07-14 13:40:00</t>
+  </si>
+  <si>
+    <t>2025-07-14 13:55:00</t>
+  </si>
+  <si>
+    <t>2025-07-14 19:30:00</t>
+  </si>
+  <si>
+    <t>線路重新接線
+測試功能正常</t>
+  </si>
+  <si>
+    <t>14259114071101</t>
+  </si>
+  <si>
+    <t>八里水灣店</t>
+  </si>
+  <si>
+    <t>新北市八里區</t>
+  </si>
+  <si>
+    <t>2025-07-11 16:57:58</t>
+  </si>
+  <si>
+    <t>無反應，不會轉動</t>
+  </si>
+  <si>
+    <t>L90-門市反應tm刷讀mmk小白單顯示印票機異常，請門市重裝紙捲重開機點選mmk偵測印票機仍異常.....須請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF04259</t>
+  </si>
+  <si>
+    <t>2025-07-11 17:00:35</t>
+  </si>
+  <si>
+    <t>2025-07-14 12:21:00</t>
+  </si>
+  <si>
+    <t>2025-07-14 12:51:00</t>
+  </si>
+  <si>
+    <t>2025-07-14 21:00:00</t>
+  </si>
+  <si>
+    <t>重新安裝紙捲測試正常，請門市在進行觀察</t>
+  </si>
+  <si>
+    <t>2025-07-14 12:23:00</t>
+  </si>
+  <si>
+    <t>2025-07-14 12:53:00</t>
+  </si>
+  <si>
+    <t>重新啟動安裝紙捲，目前測試正常，請門市在進行觀察</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> eS-4528A 黑白複合機</t>
+  </si>
+  <si>
+    <t>八里鐵塔店</t>
+  </si>
+  <si>
+    <t>THILF04528</t>
+  </si>
+  <si>
+    <t>2025-07-14 11:44:17</t>
+  </si>
+  <si>
+    <t>2025-07-14 11:10:00</t>
+  </si>
+  <si>
+    <t>2025-07-14 11:42:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PMQ3+TVV </t>
+  </si>
+  <si>
+    <t>2025-07-14 12:57:07</t>
+  </si>
+  <si>
+    <t>2025-07-14 12:20:00</t>
+  </si>
+  <si>
+    <t>2025-07-14 12:56:00</t>
+  </si>
+  <si>
+    <t>八里凱旋門</t>
+  </si>
+  <si>
+    <t>THILF02306</t>
+  </si>
+  <si>
+    <t>2025-07-14 13:16:41</t>
+  </si>
+  <si>
+    <t>2025-07-14 12:55:00</t>
+  </si>
+  <si>
+    <t>2025-07-14 13:14:00</t>
+  </si>
+  <si>
+    <t>板橋民生站</t>
+  </si>
+  <si>
+    <t>THILF05384</t>
+  </si>
+  <si>
+    <t>2025-07-14 13:31:15</t>
+  </si>
+  <si>
+    <t>2025-07-14 10:30:00</t>
+  </si>
+  <si>
+    <t>2025-07-14 13:30:00</t>
+  </si>
+  <si>
+    <t>新開門市</t>
+  </si>
+  <si>
+    <t>八里大船店</t>
+  </si>
+  <si>
+    <t>THILF04764</t>
+  </si>
+  <si>
+    <t>2025-07-14 13:48:12</t>
+  </si>
+  <si>
+    <t>2025-07-14 13:47:00</t>
+  </si>
+  <si>
+    <t>2025-07-14 13:58:16</t>
+  </si>
+  <si>
+    <t>2025-07-14 13:39:00</t>
+  </si>
+  <si>
+    <t>2025-07-14 13:54:00</t>
   </si>
 </sst>
 </file>
@@ -1725,10 +1889,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK62"/>
+  <dimension ref="A1:AK71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="AC59" sqref="AC59"/>
+      <selection activeCell="A71" sqref="A71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6807,7 +6971,7 @@
       <c r="O62" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="P62" s="4" t="s">
+      <c r="P62" s="10" t="s">
         <v>416</v>
       </c>
       <c r="Q62" s="3" t="s">
@@ -6844,7 +7008,7 @@
       <c r="AB62" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="AC62" s="4" t="s">
+      <c r="AC62" s="10" t="s">
         <v>421</v>
       </c>
       <c r="AD62" s="3"/>
@@ -6855,6 +7019,761 @@
       <c r="AI62" s="3"/>
       <c r="AJ62" s="3"/>
       <c r="AK62" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:37">
+      <c r="A63" s="7">
+        <v>61</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C63" s="7">
+        <v>2025071659</v>
+      </c>
+      <c r="D63" s="7" t="s">
+        <v>422</v>
+      </c>
+      <c r="E63" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F63" s="7">
+        <v>4167</v>
+      </c>
+      <c r="G63" s="7" t="s">
+        <v>423</v>
+      </c>
+      <c r="H63" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="I63" s="7" t="s">
+        <v>424</v>
+      </c>
+      <c r="J63" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="K63" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="L63" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="M63" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="N63" s="7">
+        <v>2307</v>
+      </c>
+      <c r="O63" s="8" t="s">
+        <v>425</v>
+      </c>
+      <c r="P63" s="9" t="s">
+        <v>426</v>
+      </c>
+      <c r="Q63" s="7" t="s">
+        <v>427</v>
+      </c>
+      <c r="R63" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S63" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="T63" s="7">
+        <v>1</v>
+      </c>
+      <c r="U63" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V63" s="7" t="s">
+        <v>428</v>
+      </c>
+      <c r="W63" s="7" t="s">
+        <v>429</v>
+      </c>
+      <c r="X63" s="7" t="s">
+        <v>430</v>
+      </c>
+      <c r="Y63" s="7" t="s">
+        <v>431</v>
+      </c>
+      <c r="Z63" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA63" s="7"/>
+      <c r="AB63" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC63" s="9" t="s">
+        <v>432</v>
+      </c>
+      <c r="AD63" s="7"/>
+      <c r="AE63" s="7"/>
+      <c r="AF63" s="7"/>
+      <c r="AG63" s="7"/>
+      <c r="AH63" s="7"/>
+      <c r="AI63" s="7"/>
+      <c r="AJ63" s="7"/>
+      <c r="AK63" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="64" spans="1:37">
+      <c r="A64" s="3">
+        <v>62</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C64" s="3">
+        <v>2025071686</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F64" s="3">
+        <v>4259</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>434</v>
+      </c>
+      <c r="H64" s="3" t="s">
+        <v>435</v>
+      </c>
+      <c r="I64" s="3" t="s">
+        <v>436</v>
+      </c>
+      <c r="J64" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="K64" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="L64" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="M64" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="N64" s="3">
+        <v>6003</v>
+      </c>
+      <c r="O64" s="4" t="s">
+        <v>437</v>
+      </c>
+      <c r="P64" s="10" t="s">
+        <v>438</v>
+      </c>
+      <c r="Q64" s="3" t="s">
+        <v>439</v>
+      </c>
+      <c r="R64" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S64" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T64" s="3">
+        <v>1</v>
+      </c>
+      <c r="U64" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V64" s="3" t="s">
+        <v>440</v>
+      </c>
+      <c r="W64" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="X64" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="Y64" s="3" t="s">
+        <v>443</v>
+      </c>
+      <c r="Z64" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA64" s="3"/>
+      <c r="AB64" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC64" s="10" t="s">
+        <v>444</v>
+      </c>
+      <c r="AD64" s="3"/>
+      <c r="AE64" s="3"/>
+      <c r="AF64" s="3"/>
+      <c r="AG64" s="3"/>
+      <c r="AH64" s="3"/>
+      <c r="AI64" s="3"/>
+      <c r="AJ64" s="3"/>
+      <c r="AK64" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="65" spans="1:37">
+      <c r="A65" s="7">
+        <v>63</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C65" s="7">
+        <v>2025071686</v>
+      </c>
+      <c r="D65" s="7" t="s">
+        <v>433</v>
+      </c>
+      <c r="E65" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F65" s="7">
+        <v>4259</v>
+      </c>
+      <c r="G65" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="H65" s="7" t="s">
+        <v>435</v>
+      </c>
+      <c r="I65" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="J65" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="K65" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="L65" s="7" t="s">
+        <v>391</v>
+      </c>
+      <c r="M65" s="8" t="s">
+        <v>392</v>
+      </c>
+      <c r="N65" s="7">
+        <v>6003</v>
+      </c>
+      <c r="O65" s="8" t="s">
+        <v>437</v>
+      </c>
+      <c r="P65" s="9" t="s">
+        <v>438</v>
+      </c>
+      <c r="Q65" s="7" t="s">
+        <v>439</v>
+      </c>
+      <c r="R65" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S65" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="T65" s="7">
+        <v>2</v>
+      </c>
+      <c r="U65" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V65" s="7" t="s">
+        <v>440</v>
+      </c>
+      <c r="W65" s="7" t="s">
+        <v>445</v>
+      </c>
+      <c r="X65" s="7" t="s">
+        <v>446</v>
+      </c>
+      <c r="Y65" s="7" t="s">
+        <v>443</v>
+      </c>
+      <c r="Z65" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA65" s="7"/>
+      <c r="AB65" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC65" s="9" t="s">
+        <v>447</v>
+      </c>
+      <c r="AD65" s="7"/>
+      <c r="AE65" s="7"/>
+      <c r="AF65" s="7"/>
+      <c r="AG65" s="7"/>
+      <c r="AH65" s="7"/>
+      <c r="AI65" s="7"/>
+      <c r="AJ65" s="7"/>
+      <c r="AK65" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="66" spans="1:37">
+      <c r="A66" s="3">
+        <v>64</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C66" s="3">
+        <v>2025071761</v>
+      </c>
+      <c r="D66" s="3"/>
+      <c r="E66" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="F66" s="3">
+        <v>4528</v>
+      </c>
+      <c r="G66" s="3" t="s">
+        <v>449</v>
+      </c>
+      <c r="H66" s="3" t="s">
+        <v>435</v>
+      </c>
+      <c r="I66" s="3"/>
+      <c r="J66" s="3"/>
+      <c r="K66" s="3"/>
+      <c r="L66" s="3"/>
+      <c r="M66" s="4"/>
+      <c r="N66" s="3"/>
+      <c r="O66" s="4"/>
+      <c r="P66" s="10"/>
+      <c r="Q66" s="3" t="s">
+        <v>450</v>
+      </c>
+      <c r="R66" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S66" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T66" s="3">
+        <v>1</v>
+      </c>
+      <c r="U66" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V66" s="3" t="s">
+        <v>451</v>
+      </c>
+      <c r="W66" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="X66" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="Y66" s="3"/>
+      <c r="Z66" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA66" s="3"/>
+      <c r="AB66" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC66" s="10" t="s">
+        <v>454</v>
+      </c>
+      <c r="AD66" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE66" s="3"/>
+      <c r="AF66" s="3"/>
+      <c r="AG66" s="3"/>
+      <c r="AH66" s="3"/>
+      <c r="AI66" s="3"/>
+      <c r="AJ66" s="3"/>
+      <c r="AK66" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="67" spans="1:37">
+      <c r="A67" s="7">
+        <v>65</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C67" s="7">
+        <v>2025071771</v>
+      </c>
+      <c r="D67" s="7"/>
+      <c r="E67" s="7"/>
+      <c r="F67" s="7">
+        <v>4259</v>
+      </c>
+      <c r="G67" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="H67" s="7" t="s">
+        <v>435</v>
+      </c>
+      <c r="I67" s="7"/>
+      <c r="J67" s="7"/>
+      <c r="K67" s="7"/>
+      <c r="L67" s="7"/>
+      <c r="M67" s="8"/>
+      <c r="N67" s="7"/>
+      <c r="O67" s="8"/>
+      <c r="P67" s="9"/>
+      <c r="Q67" s="7" t="s">
+        <v>439</v>
+      </c>
+      <c r="R67" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S67" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="T67" s="7">
+        <v>1</v>
+      </c>
+      <c r="U67" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V67" s="7" t="s">
+        <v>455</v>
+      </c>
+      <c r="W67" s="7" t="s">
+        <v>456</v>
+      </c>
+      <c r="X67" s="7" t="s">
+        <v>457</v>
+      </c>
+      <c r="Y67" s="7"/>
+      <c r="Z67" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="AA67" s="7"/>
+      <c r="AB67" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC67" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="AD67" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE67" s="7"/>
+      <c r="AF67" s="7"/>
+      <c r="AG67" s="7"/>
+      <c r="AH67" s="7"/>
+      <c r="AI67" s="7"/>
+      <c r="AJ67" s="7"/>
+      <c r="AK67" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="68" spans="1:37">
+      <c r="A68" s="3">
+        <v>66</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C68" s="3">
+        <v>2025071775</v>
+      </c>
+      <c r="D68" s="3"/>
+      <c r="E68" s="3"/>
+      <c r="F68" s="3">
+        <v>2306</v>
+      </c>
+      <c r="G68" s="3" t="s">
+        <v>458</v>
+      </c>
+      <c r="H68" s="3" t="s">
+        <v>435</v>
+      </c>
+      <c r="I68" s="3"/>
+      <c r="J68" s="3"/>
+      <c r="K68" s="3"/>
+      <c r="L68" s="3"/>
+      <c r="M68" s="4"/>
+      <c r="N68" s="3"/>
+      <c r="O68" s="4"/>
+      <c r="P68" s="10"/>
+      <c r="Q68" s="3" t="s">
+        <v>459</v>
+      </c>
+      <c r="R68" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S68" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T68" s="3">
+        <v>1</v>
+      </c>
+      <c r="U68" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V68" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="W68" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="X68" s="3" t="s">
+        <v>462</v>
+      </c>
+      <c r="Y68" s="3"/>
+      <c r="Z68" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA68" s="3"/>
+      <c r="AB68" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC68" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="AD68" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE68" s="3"/>
+      <c r="AF68" s="3"/>
+      <c r="AG68" s="3"/>
+      <c r="AH68" s="3"/>
+      <c r="AI68" s="3"/>
+      <c r="AJ68" s="3"/>
+      <c r="AK68" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="69" spans="1:37">
+      <c r="A69" s="7">
+        <v>67</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C69" s="7">
+        <v>2025071781</v>
+      </c>
+      <c r="D69" s="7"/>
+      <c r="E69" s="7"/>
+      <c r="F69" s="7">
+        <v>5384</v>
+      </c>
+      <c r="G69" s="7" t="s">
+        <v>463</v>
+      </c>
+      <c r="H69" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="I69" s="7"/>
+      <c r="J69" s="7"/>
+      <c r="K69" s="7"/>
+      <c r="L69" s="7"/>
+      <c r="M69" s="8"/>
+      <c r="N69" s="7"/>
+      <c r="O69" s="8"/>
+      <c r="P69" s="9"/>
+      <c r="Q69" s="7" t="s">
+        <v>464</v>
+      </c>
+      <c r="R69" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S69" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="T69" s="7">
+        <v>1</v>
+      </c>
+      <c r="U69" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V69" s="7" t="s">
+        <v>465</v>
+      </c>
+      <c r="W69" s="7" t="s">
+        <v>466</v>
+      </c>
+      <c r="X69" s="7" t="s">
+        <v>467</v>
+      </c>
+      <c r="Y69" s="7"/>
+      <c r="Z69" s="7">
+        <v>3</v>
+      </c>
+      <c r="AA69" s="7"/>
+      <c r="AB69" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC69" s="9" t="s">
+        <v>468</v>
+      </c>
+      <c r="AD69" s="7"/>
+      <c r="AE69" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF69" s="7"/>
+      <c r="AG69" s="7"/>
+      <c r="AH69" s="7"/>
+      <c r="AI69" s="7"/>
+      <c r="AJ69" s="7"/>
+      <c r="AK69" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="70" spans="1:37">
+      <c r="A70" s="3">
+        <v>68</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C70" s="3">
+        <v>2025071785</v>
+      </c>
+      <c r="D70" s="3"/>
+      <c r="E70" s="3"/>
+      <c r="F70" s="3">
+        <v>4764</v>
+      </c>
+      <c r="G70" s="3" t="s">
+        <v>469</v>
+      </c>
+      <c r="H70" s="3" t="s">
+        <v>435</v>
+      </c>
+      <c r="I70" s="3"/>
+      <c r="J70" s="3"/>
+      <c r="K70" s="3"/>
+      <c r="L70" s="3"/>
+      <c r="M70" s="4"/>
+      <c r="N70" s="3"/>
+      <c r="O70" s="4"/>
+      <c r="P70" s="10"/>
+      <c r="Q70" s="3" t="s">
+        <v>470</v>
+      </c>
+      <c r="R70" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S70" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T70" s="3">
+        <v>1</v>
+      </c>
+      <c r="U70" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V70" s="3" t="s">
+        <v>471</v>
+      </c>
+      <c r="W70" s="3" t="s">
+        <v>467</v>
+      </c>
+      <c r="X70" s="3" t="s">
+        <v>472</v>
+      </c>
+      <c r="Y70" s="3"/>
+      <c r="Z70" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA70" s="3"/>
+      <c r="AB70" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC70" s="10" t="s">
+        <v>355</v>
+      </c>
+      <c r="AD70" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE70" s="3"/>
+      <c r="AF70" s="3"/>
+      <c r="AG70" s="3"/>
+      <c r="AH70" s="3"/>
+      <c r="AI70" s="3"/>
+      <c r="AJ70" s="3"/>
+      <c r="AK70" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="71" spans="1:37">
+      <c r="A71" s="7">
+        <v>69</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C71" s="7">
+        <v>2025071789</v>
+      </c>
+      <c r="D71" s="7"/>
+      <c r="E71" s="7"/>
+      <c r="F71" s="7">
+        <v>4167</v>
+      </c>
+      <c r="G71" s="7" t="s">
+        <v>423</v>
+      </c>
+      <c r="H71" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="I71" s="7"/>
+      <c r="J71" s="7"/>
+      <c r="K71" s="7"/>
+      <c r="L71" s="7"/>
+      <c r="M71" s="8"/>
+      <c r="N71" s="7"/>
+      <c r="O71" s="8"/>
+      <c r="P71" s="8"/>
+      <c r="Q71" s="7" t="s">
+        <v>427</v>
+      </c>
+      <c r="R71" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S71" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="T71" s="7">
+        <v>1</v>
+      </c>
+      <c r="U71" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V71" s="7" t="s">
+        <v>473</v>
+      </c>
+      <c r="W71" s="7" t="s">
+        <v>474</v>
+      </c>
+      <c r="X71" s="7" t="s">
+        <v>475</v>
+      </c>
+      <c r="Y71" s="7"/>
+      <c r="Z71" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA71" s="7"/>
+      <c r="AB71" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC71" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="AD71" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE71" s="7"/>
+      <c r="AF71" s="7"/>
+      <c r="AG71" s="7"/>
+      <c r="AH71" s="7"/>
+      <c r="AI71" s="7"/>
+      <c r="AJ71" s="7"/>
+      <c r="AK71" s="7" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit on 21-2025-time
</commit_message>
<xml_diff>
--- a/IM/202507_HL_Maintain_Report.xlsx
+++ b/IM/202507_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$85</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$86</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="564">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202507   (  製表日期:2025-07-18  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="569">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202507   (  製表日期:2025-07-21  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -1747,6 +1747,21 @@
   </si>
   <si>
     <t>2025-07-18 11:30:00</t>
+  </si>
+  <si>
+    <t>新莊小胖店</t>
+  </si>
+  <si>
+    <t>THILF04856</t>
+  </si>
+  <si>
+    <t>2025-07-21 11:35:28</t>
+  </si>
+  <si>
+    <t>2025-07-21 11:10:00</t>
+  </si>
+  <si>
+    <t>2025-07-21 11:30:00</t>
   </si>
 </sst>
 </file>
@@ -2160,10 +2175,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK85"/>
+  <dimension ref="A1:AK86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A85" sqref="A85"/>
+      <selection activeCell="AC83" sqref="AC83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9177,7 +9192,7 @@
       <c r="M85" s="8"/>
       <c r="N85" s="7"/>
       <c r="O85" s="8"/>
-      <c r="P85" s="8"/>
+      <c r="P85" s="9"/>
       <c r="Q85" s="7" t="s">
         <v>548</v>
       </c>
@@ -9210,7 +9225,7 @@
       <c r="AB85" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="AC85" s="8" t="s">
+      <c r="AC85" s="9" t="s">
         <v>95</v>
       </c>
       <c r="AD85" s="7" t="s">
@@ -9223,6 +9238,83 @@
       <c r="AI85" s="7"/>
       <c r="AJ85" s="7"/>
       <c r="AK85" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="86" spans="1:37">
+      <c r="A86" s="3">
+        <v>84</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C86" s="3">
+        <v>2025072592</v>
+      </c>
+      <c r="D86" s="3"/>
+      <c r="E86" s="3"/>
+      <c r="F86" s="3">
+        <v>4856</v>
+      </c>
+      <c r="G86" s="3" t="s">
+        <v>564</v>
+      </c>
+      <c r="H86" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="I86" s="3"/>
+      <c r="J86" s="3"/>
+      <c r="K86" s="3"/>
+      <c r="L86" s="3"/>
+      <c r="M86" s="4"/>
+      <c r="N86" s="3"/>
+      <c r="O86" s="4"/>
+      <c r="P86" s="4"/>
+      <c r="Q86" s="3" t="s">
+        <v>565</v>
+      </c>
+      <c r="R86" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S86" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="T86" s="3">
+        <v>1</v>
+      </c>
+      <c r="U86" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V86" s="3" t="s">
+        <v>566</v>
+      </c>
+      <c r="W86" s="3" t="s">
+        <v>567</v>
+      </c>
+      <c r="X86" s="3" t="s">
+        <v>568</v>
+      </c>
+      <c r="Y86" s="3"/>
+      <c r="Z86" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA86" s="3"/>
+      <c r="AB86" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC86" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="AD86" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE86" s="3"/>
+      <c r="AF86" s="3"/>
+      <c r="AG86" s="3"/>
+      <c r="AH86" s="3"/>
+      <c r="AI86" s="3"/>
+      <c r="AJ86" s="3"/>
+      <c r="AK86" s="3" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit on 22-2025-time
</commit_message>
<xml_diff>
--- a/IM/202507_HL_Maintain_Report.xlsx
+++ b/IM/202507_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$86</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$93</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="569">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202507   (  製表日期:2025-07-21  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="620">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202507   (  製表日期:2025-07-22  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -1749,6 +1749,69 @@
     <t>2025-07-18 11:30:00</t>
   </si>
   <si>
+    <t>14167114071901</t>
+  </si>
+  <si>
+    <t>2025-07-19 10:57:58</t>
+  </si>
+  <si>
+    <t>HLF6</t>
+  </si>
+  <si>
+    <t>HL-多卡機QP3000E</t>
+  </si>
+  <si>
+    <t>F604</t>
+  </si>
+  <si>
+    <t>無電源反應</t>
+  </si>
+  <si>
+    <t>門市反應tm1多卡機(QP3000E)無法使用無畫面無電源反應，門市已重新拔插後方線路仍異常....須請台芝到店協助</t>
+  </si>
+  <si>
+    <t>2025-07-19 10:59:08</t>
+  </si>
+  <si>
+    <t>2025-07-22 11:03:00</t>
+  </si>
+  <si>
+    <t>2025-07-22 11:35:00</t>
+  </si>
+  <si>
+    <t>2025-07-22 13:00:00</t>
+  </si>
+  <si>
+    <t>更換QP3000
+換上：8183000557
+換下：8183001946</t>
+  </si>
+  <si>
+    <t>14196114072101</t>
+  </si>
+  <si>
+    <t>2025-07-21 10:35:51</t>
+  </si>
+  <si>
+    <t>TM2-CCD掃描器(HC56II-TR)-門市反應於TM2操作菸品交易，點選提醒視窗是後，再次刷讀商品會無反應，都需在面板多點幾次再刷讀才有反應，已嘗試執行TM2觸控校正、TM2-CCD掃描器校正仍無改善，且發現不只菸品，大部分的商品條碼都感應不靈敏，台芝於07/03更換過掃描器門市告知更換完一段時間皆正常，但近期又發生且刷讀所有商品條碼都會有此狀況，門市已有操作校正仍異常..請台芝到店協助</t>
+  </si>
+  <si>
+    <t>2025-07-21 10:38:46</t>
+  </si>
+  <si>
+    <t>2025-07-22 10:40:00</t>
+  </si>
+  <si>
+    <t>2025-07-22 12:04:00</t>
+  </si>
+  <si>
+    <t>2025-07-22 14:38:00</t>
+  </si>
+  <si>
+    <t>TM2因為經常刷商品會突發性刷讀不到，點畫面也無法解決，這問題在7/2換過新的掃槍到現在店員反應依然無改善狀況
+先與TM1 com線做交換測試，請店員在進行觀察，先進行排除是否com線問題</t>
+  </si>
+  <si>
     <t>新莊小胖店</t>
   </si>
   <si>
@@ -1762,6 +1825,100 @@
   </si>
   <si>
     <t>2025-07-21 11:30:00</t>
+  </si>
+  <si>
+    <t>新莊福祐店</t>
+  </si>
+  <si>
+    <t>THILF03999</t>
+  </si>
+  <si>
+    <t>2025-07-21 14:32:19</t>
+  </si>
+  <si>
+    <t>2025-07-21 14:00:00</t>
+  </si>
+  <si>
+    <t>2025-07-21 14:40:00</t>
+  </si>
+  <si>
+    <t>暫撤</t>
+  </si>
+  <si>
+    <t>E4260114072201</t>
+  </si>
+  <si>
+    <t>2025-07-22 09:21:05</t>
+  </si>
+  <si>
+    <t>門市反應tm2(TCX800)觸控異常鼠標閃爍會一直亂跳，vnc查看鼠標亂跑無法操作校正重啟後可操作螢幕觸控校正，校正後門市使用仍異常....須請台芝到店協助(機2的鼠飆往右下偏移)</t>
+  </si>
+  <si>
+    <t>2025-07-22 09:54:48</t>
+  </si>
+  <si>
+    <t>2025-07-22 12:26:00</t>
+  </si>
+  <si>
+    <t>2025-07-22 12:56:00</t>
+  </si>
+  <si>
+    <t>2025-07-23 13:54:00</t>
+  </si>
+  <si>
+    <t>重新矯正螢幕，目前測試正常</t>
+  </si>
+  <si>
+    <t>1D111114072201</t>
+  </si>
+  <si>
+    <t>D111</t>
+  </si>
+  <si>
+    <t>北縣府中店</t>
+  </si>
+  <si>
+    <t>2025-07-22 11:24:10</t>
+  </si>
+  <si>
+    <t>HL59</t>
+  </si>
+  <si>
+    <t>HL-LIFE-ET熱感機T70II</t>
+  </si>
+  <si>
+    <t>門市反應LIFEET熱感機T70II error亮橘燈，於LIFEET操作列印測試票券小白單無法列印，畫面下方有顯示印表機離線，已有關機紙捲重裝仍異常...請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF0D111</t>
+  </si>
+  <si>
+    <t>2025-07-22 11:26:34</t>
+  </si>
+  <si>
+    <t>2025-07-22 11:45:00</t>
+  </si>
+  <si>
+    <t>2025-07-22 12:35:00</t>
+  </si>
+  <si>
+    <t>2025-07-23 15:26:00</t>
+  </si>
+  <si>
+    <t>內部清潔後
+測試正常</t>
+  </si>
+  <si>
+    <t>2025-07-22 12:38:11</t>
+  </si>
+  <si>
+    <t>2025-07-22 12:59:05</t>
+  </si>
+  <si>
+    <t>2025-07-22 12:43:00</t>
+  </si>
+  <si>
+    <t>2025-07-22 12:58:00</t>
   </si>
 </sst>
 </file>
@@ -2175,10 +2332,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK86"/>
+  <dimension ref="A1:AK93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="AC83" sqref="AC83"/>
+      <selection activeCell="A93" sqref="A93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9246,38 +9403,58 @@
         <v>84</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>87</v>
+        <v>38</v>
       </c>
       <c r="C86" s="3">
-        <v>2025072592</v>
-      </c>
-      <c r="D86" s="3"/>
-      <c r="E86" s="3"/>
+        <v>2025072526</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>564</v>
+      </c>
+      <c r="E86" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="F86" s="3">
-        <v>4856</v>
+        <v>4167</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>564</v>
+        <v>423</v>
       </c>
       <c r="H86" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="I86" s="3"/>
-      <c r="J86" s="3"/>
-      <c r="K86" s="3"/>
-      <c r="L86" s="3"/>
-      <c r="M86" s="4"/>
-      <c r="N86" s="3"/>
-      <c r="O86" s="4"/>
-      <c r="P86" s="4"/>
+        <v>64</v>
+      </c>
+      <c r="I86" s="3" t="s">
+        <v>565</v>
+      </c>
+      <c r="J86" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="K86" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="L86" s="3" t="s">
+        <v>566</v>
+      </c>
+      <c r="M86" s="4" t="s">
+        <v>567</v>
+      </c>
+      <c r="N86" s="3" t="s">
+        <v>568</v>
+      </c>
+      <c r="O86" s="4" t="s">
+        <v>569</v>
+      </c>
+      <c r="P86" s="10" t="s">
+        <v>570</v>
+      </c>
       <c r="Q86" s="3" t="s">
-        <v>565</v>
+        <v>427</v>
       </c>
       <c r="R86" s="3" t="s">
         <v>52</v>
       </c>
       <c r="S86" s="3" t="s">
-        <v>136</v>
+        <v>74</v>
       </c>
       <c r="T86" s="3">
         <v>1</v>
@@ -9286,28 +9463,28 @@
         <v>54</v>
       </c>
       <c r="V86" s="3" t="s">
-        <v>566</v>
+        <v>571</v>
       </c>
       <c r="W86" s="3" t="s">
-        <v>567</v>
+        <v>572</v>
       </c>
       <c r="X86" s="3" t="s">
-        <v>568</v>
-      </c>
-      <c r="Y86" s="3"/>
+        <v>573</v>
+      </c>
+      <c r="Y86" s="3" t="s">
+        <v>574</v>
+      </c>
       <c r="Z86" s="3">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="AA86" s="3"/>
       <c r="AB86" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="AC86" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="AD86" s="3" t="s">
-        <v>61</v>
-      </c>
+      <c r="AC86" s="10" t="s">
+        <v>575</v>
+      </c>
+      <c r="AD86" s="3"/>
       <c r="AE86" s="3"/>
       <c r="AF86" s="3"/>
       <c r="AG86" s="3"/>
@@ -9315,6 +9492,605 @@
       <c r="AI86" s="3"/>
       <c r="AJ86" s="3"/>
       <c r="AK86" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="87" spans="1:37">
+      <c r="A87" s="7">
+        <v>85</v>
+      </c>
+      <c r="B87" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C87" s="7">
+        <v>2025072574</v>
+      </c>
+      <c r="D87" s="7" t="s">
+        <v>576</v>
+      </c>
+      <c r="E87" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F87" s="7">
+        <v>4196</v>
+      </c>
+      <c r="G87" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="H87" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I87" s="7" t="s">
+        <v>577</v>
+      </c>
+      <c r="J87" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="K87" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="L87" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="M87" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="N87" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="O87" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="P87" s="9" t="s">
+        <v>578</v>
+      </c>
+      <c r="Q87" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="R87" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S87" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="T87" s="7">
+        <v>1</v>
+      </c>
+      <c r="U87" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V87" s="7" t="s">
+        <v>579</v>
+      </c>
+      <c r="W87" s="7" t="s">
+        <v>580</v>
+      </c>
+      <c r="X87" s="7" t="s">
+        <v>581</v>
+      </c>
+      <c r="Y87" s="7" t="s">
+        <v>582</v>
+      </c>
+      <c r="Z87" s="7">
+        <v>1.4</v>
+      </c>
+      <c r="AA87" s="7"/>
+      <c r="AB87" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC87" s="9" t="s">
+        <v>583</v>
+      </c>
+      <c r="AD87" s="7"/>
+      <c r="AE87" s="7"/>
+      <c r="AF87" s="7"/>
+      <c r="AG87" s="7"/>
+      <c r="AH87" s="7"/>
+      <c r="AI87" s="7"/>
+      <c r="AJ87" s="7"/>
+      <c r="AK87" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="88" spans="1:37">
+      <c r="A88" s="3">
+        <v>86</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C88" s="3">
+        <v>2025072592</v>
+      </c>
+      <c r="D88" s="3"/>
+      <c r="E88" s="3"/>
+      <c r="F88" s="3">
+        <v>4856</v>
+      </c>
+      <c r="G88" s="3" t="s">
+        <v>584</v>
+      </c>
+      <c r="H88" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="I88" s="3"/>
+      <c r="J88" s="3"/>
+      <c r="K88" s="3"/>
+      <c r="L88" s="3"/>
+      <c r="M88" s="4"/>
+      <c r="N88" s="3"/>
+      <c r="O88" s="4"/>
+      <c r="P88" s="10"/>
+      <c r="Q88" s="3" t="s">
+        <v>585</v>
+      </c>
+      <c r="R88" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S88" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="T88" s="3">
+        <v>1</v>
+      </c>
+      <c r="U88" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V88" s="3" t="s">
+        <v>586</v>
+      </c>
+      <c r="W88" s="3" t="s">
+        <v>587</v>
+      </c>
+      <c r="X88" s="3" t="s">
+        <v>588</v>
+      </c>
+      <c r="Y88" s="3"/>
+      <c r="Z88" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA88" s="3"/>
+      <c r="AB88" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC88" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="AD88" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE88" s="3"/>
+      <c r="AF88" s="3"/>
+      <c r="AG88" s="3"/>
+      <c r="AH88" s="3"/>
+      <c r="AI88" s="3"/>
+      <c r="AJ88" s="3"/>
+      <c r="AK88" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="89" spans="1:37">
+      <c r="A89" s="7">
+        <v>87</v>
+      </c>
+      <c r="B89" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C89" s="7">
+        <v>2025072661</v>
+      </c>
+      <c r="D89" s="7"/>
+      <c r="E89" s="7"/>
+      <c r="F89" s="7">
+        <v>3999</v>
+      </c>
+      <c r="G89" s="7" t="s">
+        <v>589</v>
+      </c>
+      <c r="H89" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="I89" s="7"/>
+      <c r="J89" s="7"/>
+      <c r="K89" s="7"/>
+      <c r="L89" s="7"/>
+      <c r="M89" s="8"/>
+      <c r="N89" s="7"/>
+      <c r="O89" s="8"/>
+      <c r="P89" s="9"/>
+      <c r="Q89" s="7" t="s">
+        <v>590</v>
+      </c>
+      <c r="R89" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S89" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="T89" s="7">
+        <v>1</v>
+      </c>
+      <c r="U89" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V89" s="7" t="s">
+        <v>591</v>
+      </c>
+      <c r="W89" s="7" t="s">
+        <v>592</v>
+      </c>
+      <c r="X89" s="7" t="s">
+        <v>593</v>
+      </c>
+      <c r="Y89" s="7"/>
+      <c r="Z89" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="AA89" s="7"/>
+      <c r="AB89" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC89" s="9" t="s">
+        <v>594</v>
+      </c>
+      <c r="AD89" s="7"/>
+      <c r="AE89" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF89" s="7"/>
+      <c r="AG89" s="7"/>
+      <c r="AH89" s="7"/>
+      <c r="AI89" s="7"/>
+      <c r="AJ89" s="7"/>
+      <c r="AK89" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="90" spans="1:37">
+      <c r="A90" s="3">
+        <v>88</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C90" s="3">
+        <v>2025072752</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>595</v>
+      </c>
+      <c r="E90" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F90" s="3">
+        <v>4260</v>
+      </c>
+      <c r="G90" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H90" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I90" s="3" t="s">
+        <v>596</v>
+      </c>
+      <c r="J90" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="K90" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="L90" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="M90" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="N90" s="3">
+        <v>2307</v>
+      </c>
+      <c r="O90" s="4" t="s">
+        <v>425</v>
+      </c>
+      <c r="P90" s="10" t="s">
+        <v>597</v>
+      </c>
+      <c r="Q90" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="R90" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S90" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T90" s="3">
+        <v>1</v>
+      </c>
+      <c r="U90" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V90" s="3" t="s">
+        <v>598</v>
+      </c>
+      <c r="W90" s="3" t="s">
+        <v>599</v>
+      </c>
+      <c r="X90" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="Y90" s="3" t="s">
+        <v>601</v>
+      </c>
+      <c r="Z90" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA90" s="3"/>
+      <c r="AB90" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC90" s="10" t="s">
+        <v>602</v>
+      </c>
+      <c r="AD90" s="3"/>
+      <c r="AE90" s="3"/>
+      <c r="AF90" s="3"/>
+      <c r="AG90" s="3"/>
+      <c r="AH90" s="3"/>
+      <c r="AI90" s="3"/>
+      <c r="AJ90" s="3"/>
+      <c r="AK90" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="91" spans="1:37">
+      <c r="A91" s="7">
+        <v>89</v>
+      </c>
+      <c r="B91" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C91" s="7">
+        <v>2025072799</v>
+      </c>
+      <c r="D91" s="7" t="s">
+        <v>603</v>
+      </c>
+      <c r="E91" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F91" s="7" t="s">
+        <v>604</v>
+      </c>
+      <c r="G91" s="7" t="s">
+        <v>605</v>
+      </c>
+      <c r="H91" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="I91" s="7" t="s">
+        <v>606</v>
+      </c>
+      <c r="J91" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="K91" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="L91" s="7" t="s">
+        <v>607</v>
+      </c>
+      <c r="M91" s="8" t="s">
+        <v>608</v>
+      </c>
+      <c r="N91" s="7">
+        <v>5903</v>
+      </c>
+      <c r="O91" s="8" t="s">
+        <v>437</v>
+      </c>
+      <c r="P91" s="9" t="s">
+        <v>609</v>
+      </c>
+      <c r="Q91" s="7" t="s">
+        <v>610</v>
+      </c>
+      <c r="R91" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S91" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="T91" s="7">
+        <v>1</v>
+      </c>
+      <c r="U91" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V91" s="7" t="s">
+        <v>611</v>
+      </c>
+      <c r="W91" s="7" t="s">
+        <v>612</v>
+      </c>
+      <c r="X91" s="7" t="s">
+        <v>613</v>
+      </c>
+      <c r="Y91" s="7" t="s">
+        <v>614</v>
+      </c>
+      <c r="Z91" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="AA91" s="7"/>
+      <c r="AB91" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC91" s="9" t="s">
+        <v>615</v>
+      </c>
+      <c r="AD91" s="7"/>
+      <c r="AE91" s="7"/>
+      <c r="AF91" s="7"/>
+      <c r="AG91" s="7"/>
+      <c r="AH91" s="7"/>
+      <c r="AI91" s="7"/>
+      <c r="AJ91" s="7"/>
+      <c r="AK91" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="92" spans="1:37">
+      <c r="A92" s="3">
+        <v>90</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C92" s="3">
+        <v>2025072819</v>
+      </c>
+      <c r="D92" s="3"/>
+      <c r="E92" s="3"/>
+      <c r="F92" s="3" t="s">
+        <v>604</v>
+      </c>
+      <c r="G92" s="3" t="s">
+        <v>605</v>
+      </c>
+      <c r="H92" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I92" s="3"/>
+      <c r="J92" s="3"/>
+      <c r="K92" s="3"/>
+      <c r="L92" s="3"/>
+      <c r="M92" s="4"/>
+      <c r="N92" s="3"/>
+      <c r="O92" s="4"/>
+      <c r="P92" s="10"/>
+      <c r="Q92" s="3" t="s">
+        <v>610</v>
+      </c>
+      <c r="R92" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S92" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="T92" s="3">
+        <v>1</v>
+      </c>
+      <c r="U92" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V92" s="3" t="s">
+        <v>616</v>
+      </c>
+      <c r="W92" s="3" t="s">
+        <v>612</v>
+      </c>
+      <c r="X92" s="3" t="s">
+        <v>613</v>
+      </c>
+      <c r="Y92" s="3"/>
+      <c r="Z92" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="AA92" s="3"/>
+      <c r="AB92" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC92" s="10" t="s">
+        <v>355</v>
+      </c>
+      <c r="AD92" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE92" s="3"/>
+      <c r="AF92" s="3"/>
+      <c r="AG92" s="3"/>
+      <c r="AH92" s="3"/>
+      <c r="AI92" s="3"/>
+      <c r="AJ92" s="3"/>
+      <c r="AK92" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="93" spans="1:37">
+      <c r="A93" s="7">
+        <v>91</v>
+      </c>
+      <c r="B93" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C93" s="7">
+        <v>2025072821</v>
+      </c>
+      <c r="D93" s="7"/>
+      <c r="E93" s="7"/>
+      <c r="F93" s="7">
+        <v>4260</v>
+      </c>
+      <c r="G93" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H93" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I93" s="7"/>
+      <c r="J93" s="7"/>
+      <c r="K93" s="7"/>
+      <c r="L93" s="7"/>
+      <c r="M93" s="8"/>
+      <c r="N93" s="7"/>
+      <c r="O93" s="8"/>
+      <c r="P93" s="8"/>
+      <c r="Q93" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="R93" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S93" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="T93" s="7">
+        <v>1</v>
+      </c>
+      <c r="U93" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V93" s="7" t="s">
+        <v>617</v>
+      </c>
+      <c r="W93" s="7" t="s">
+        <v>618</v>
+      </c>
+      <c r="X93" s="7" t="s">
+        <v>619</v>
+      </c>
+      <c r="Y93" s="7"/>
+      <c r="Z93" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA93" s="7"/>
+      <c r="AB93" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC93" s="8" t="s">
+        <v>355</v>
+      </c>
+      <c r="AD93" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE93" s="7"/>
+      <c r="AF93" s="7"/>
+      <c r="AG93" s="7"/>
+      <c r="AH93" s="7"/>
+      <c r="AI93" s="7"/>
+      <c r="AJ93" s="7"/>
+      <c r="AK93" s="7" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit on 28-2025-time
</commit_message>
<xml_diff>
--- a/IM/202507_HL_Maintain_Report.xlsx
+++ b/IM/202507_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$114</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$121</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="754">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202507   (  製表日期:2025-07-25  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="789">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202507   (  製表日期:2025-07-28  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -2340,6 +2340,111 @@
   </si>
   <si>
     <t>撤機</t>
+  </si>
+  <si>
+    <t>三重星光店</t>
+  </si>
+  <si>
+    <t>THILF03983</t>
+  </si>
+  <si>
+    <t>2025-07-28 11:27:14</t>
+  </si>
+  <si>
+    <t>2025-07-28 11:00:00</t>
+  </si>
+  <si>
+    <t>2025-07-28 11:26:00</t>
+  </si>
+  <si>
+    <t>三重國隆店</t>
+  </si>
+  <si>
+    <t>THILF04804</t>
+  </si>
+  <si>
+    <t>2025-07-28 12:52:51</t>
+  </si>
+  <si>
+    <t>2025-07-28 11:32:00</t>
+  </si>
+  <si>
+    <t>2025-07-28 11:47:00</t>
+  </si>
+  <si>
+    <t>三重文化北</t>
+  </si>
+  <si>
+    <t>THILF04312</t>
+  </si>
+  <si>
+    <t>2025-07-28 12:53:36</t>
+  </si>
+  <si>
+    <t>2025-07-28 12:30:00</t>
+  </si>
+  <si>
+    <t>2025-07-28 12:52:00</t>
+  </si>
+  <si>
+    <t>三重大榮店</t>
+  </si>
+  <si>
+    <t>THILF02619</t>
+  </si>
+  <si>
+    <t>2025-07-28 13:16:37</t>
+  </si>
+  <si>
+    <t>2025-07-28 13:00:00</t>
+  </si>
+  <si>
+    <t>2025-07-28 13:15:00</t>
+  </si>
+  <si>
+    <t>三重夜市口</t>
+  </si>
+  <si>
+    <t>THILF02935</t>
+  </si>
+  <si>
+    <t>2025-07-28 14:02:43</t>
+  </si>
+  <si>
+    <t>2025-07-28 13:40:00</t>
+  </si>
+  <si>
+    <t>2025-07-28 14:02:00</t>
+  </si>
+  <si>
+    <t>新莊瓊泰店</t>
+  </si>
+  <si>
+    <t>THILF04208</t>
+  </si>
+  <si>
+    <t>2025-07-28 15:03:51</t>
+  </si>
+  <si>
+    <t>2025-07-28 14:55:00</t>
+  </si>
+  <si>
+    <t>2025-07-28 15:10:00</t>
+  </si>
+  <si>
+    <t>三重中央南</t>
+  </si>
+  <si>
+    <t>THILF04083</t>
+  </si>
+  <si>
+    <t>2025-07-28 15:04:16</t>
+  </si>
+  <si>
+    <t>2025-07-28 14:40:00</t>
+  </si>
+  <si>
+    <t>2025-07-28 15:03:00</t>
   </si>
 </sst>
 </file>
@@ -2753,10 +2858,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK114"/>
+  <dimension ref="A1:AK121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="AC111" sqref="AC111"/>
+      <selection activeCell="A121" sqref="A121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12263,7 +12368,7 @@
       <c r="M114" s="4"/>
       <c r="N114" s="3"/>
       <c r="O114" s="4"/>
-      <c r="P114" s="4"/>
+      <c r="P114" s="10"/>
       <c r="Q114" s="3" t="s">
         <v>749</v>
       </c>
@@ -12296,7 +12401,7 @@
       <c r="AB114" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="AC114" s="4" t="s">
+      <c r="AC114" s="10" t="s">
         <v>753</v>
       </c>
       <c r="AD114" s="3"/>
@@ -12309,6 +12414,545 @@
       <c r="AI114" s="3"/>
       <c r="AJ114" s="3"/>
       <c r="AK114" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="115" spans="1:37">
+      <c r="A115" s="7">
+        <v>113</v>
+      </c>
+      <c r="B115" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C115" s="7">
+        <v>2025073528</v>
+      </c>
+      <c r="D115" s="7"/>
+      <c r="E115" s="7"/>
+      <c r="F115" s="7">
+        <v>3983</v>
+      </c>
+      <c r="G115" s="7" t="s">
+        <v>754</v>
+      </c>
+      <c r="H115" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I115" s="7"/>
+      <c r="J115" s="7"/>
+      <c r="K115" s="7"/>
+      <c r="L115" s="7"/>
+      <c r="M115" s="8"/>
+      <c r="N115" s="7"/>
+      <c r="O115" s="8"/>
+      <c r="P115" s="9"/>
+      <c r="Q115" s="7" t="s">
+        <v>755</v>
+      </c>
+      <c r="R115" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S115" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="T115" s="7">
+        <v>1</v>
+      </c>
+      <c r="U115" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V115" s="7" t="s">
+        <v>756</v>
+      </c>
+      <c r="W115" s="7" t="s">
+        <v>757</v>
+      </c>
+      <c r="X115" s="7" t="s">
+        <v>758</v>
+      </c>
+      <c r="Y115" s="7"/>
+      <c r="Z115" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="AA115" s="7"/>
+      <c r="AB115" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC115" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="AD115" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE115" s="7"/>
+      <c r="AF115" s="7"/>
+      <c r="AG115" s="7"/>
+      <c r="AH115" s="7"/>
+      <c r="AI115" s="7"/>
+      <c r="AJ115" s="7"/>
+      <c r="AK115" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="116" spans="1:37">
+      <c r="A116" s="3">
+        <v>114</v>
+      </c>
+      <c r="B116" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C116" s="3">
+        <v>2025073542</v>
+      </c>
+      <c r="D116" s="3"/>
+      <c r="E116" s="3"/>
+      <c r="F116" s="3">
+        <v>4804</v>
+      </c>
+      <c r="G116" s="3" t="s">
+        <v>759</v>
+      </c>
+      <c r="H116" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I116" s="3"/>
+      <c r="J116" s="3"/>
+      <c r="K116" s="3"/>
+      <c r="L116" s="3"/>
+      <c r="M116" s="4"/>
+      <c r="N116" s="3"/>
+      <c r="O116" s="4"/>
+      <c r="P116" s="10"/>
+      <c r="Q116" s="3" t="s">
+        <v>760</v>
+      </c>
+      <c r="R116" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S116" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T116" s="3">
+        <v>1</v>
+      </c>
+      <c r="U116" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V116" s="3" t="s">
+        <v>761</v>
+      </c>
+      <c r="W116" s="3" t="s">
+        <v>762</v>
+      </c>
+      <c r="X116" s="3" t="s">
+        <v>763</v>
+      </c>
+      <c r="Y116" s="3"/>
+      <c r="Z116" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA116" s="3"/>
+      <c r="AB116" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC116" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="AD116" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE116" s="3"/>
+      <c r="AF116" s="3"/>
+      <c r="AG116" s="3"/>
+      <c r="AH116" s="3"/>
+      <c r="AI116" s="3"/>
+      <c r="AJ116" s="3"/>
+      <c r="AK116" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="117" spans="1:37">
+      <c r="A117" s="7">
+        <v>115</v>
+      </c>
+      <c r="B117" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C117" s="7">
+        <v>2025073543</v>
+      </c>
+      <c r="D117" s="7"/>
+      <c r="E117" s="7"/>
+      <c r="F117" s="7">
+        <v>4312</v>
+      </c>
+      <c r="G117" s="7" t="s">
+        <v>764</v>
+      </c>
+      <c r="H117" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I117" s="7"/>
+      <c r="J117" s="7"/>
+      <c r="K117" s="7"/>
+      <c r="L117" s="7"/>
+      <c r="M117" s="8"/>
+      <c r="N117" s="7"/>
+      <c r="O117" s="8"/>
+      <c r="P117" s="9"/>
+      <c r="Q117" s="7" t="s">
+        <v>765</v>
+      </c>
+      <c r="R117" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S117" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="T117" s="7">
+        <v>1</v>
+      </c>
+      <c r="U117" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V117" s="7" t="s">
+        <v>766</v>
+      </c>
+      <c r="W117" s="7" t="s">
+        <v>767</v>
+      </c>
+      <c r="X117" s="7" t="s">
+        <v>768</v>
+      </c>
+      <c r="Y117" s="7"/>
+      <c r="Z117" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="AA117" s="7"/>
+      <c r="AB117" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC117" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="AD117" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE117" s="7"/>
+      <c r="AF117" s="7"/>
+      <c r="AG117" s="7"/>
+      <c r="AH117" s="7"/>
+      <c r="AI117" s="7"/>
+      <c r="AJ117" s="7"/>
+      <c r="AK117" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="118" spans="1:37">
+      <c r="A118" s="3">
+        <v>116</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C118" s="3">
+        <v>2025073544</v>
+      </c>
+      <c r="D118" s="3"/>
+      <c r="E118" s="3"/>
+      <c r="F118" s="3">
+        <v>2619</v>
+      </c>
+      <c r="G118" s="3" t="s">
+        <v>769</v>
+      </c>
+      <c r="H118" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I118" s="3"/>
+      <c r="J118" s="3"/>
+      <c r="K118" s="3"/>
+      <c r="L118" s="3"/>
+      <c r="M118" s="4"/>
+      <c r="N118" s="3"/>
+      <c r="O118" s="4"/>
+      <c r="P118" s="10"/>
+      <c r="Q118" s="3" t="s">
+        <v>770</v>
+      </c>
+      <c r="R118" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S118" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T118" s="3">
+        <v>1</v>
+      </c>
+      <c r="U118" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V118" s="3" t="s">
+        <v>771</v>
+      </c>
+      <c r="W118" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="X118" s="3" t="s">
+        <v>773</v>
+      </c>
+      <c r="Y118" s="3"/>
+      <c r="Z118" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA118" s="3"/>
+      <c r="AB118" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC118" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="AD118" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE118" s="3"/>
+      <c r="AF118" s="3"/>
+      <c r="AG118" s="3"/>
+      <c r="AH118" s="3"/>
+      <c r="AI118" s="3"/>
+      <c r="AJ118" s="3"/>
+      <c r="AK118" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="119" spans="1:37">
+      <c r="A119" s="7">
+        <v>117</v>
+      </c>
+      <c r="B119" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C119" s="7">
+        <v>2025073555</v>
+      </c>
+      <c r="D119" s="7"/>
+      <c r="E119" s="7"/>
+      <c r="F119" s="7">
+        <v>2935</v>
+      </c>
+      <c r="G119" s="7" t="s">
+        <v>774</v>
+      </c>
+      <c r="H119" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I119" s="7"/>
+      <c r="J119" s="7"/>
+      <c r="K119" s="7"/>
+      <c r="L119" s="7"/>
+      <c r="M119" s="8"/>
+      <c r="N119" s="7"/>
+      <c r="O119" s="8"/>
+      <c r="P119" s="9"/>
+      <c r="Q119" s="7" t="s">
+        <v>775</v>
+      </c>
+      <c r="R119" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S119" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="T119" s="7">
+        <v>1</v>
+      </c>
+      <c r="U119" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V119" s="7" t="s">
+        <v>776</v>
+      </c>
+      <c r="W119" s="7" t="s">
+        <v>777</v>
+      </c>
+      <c r="X119" s="7" t="s">
+        <v>778</v>
+      </c>
+      <c r="Y119" s="7"/>
+      <c r="Z119" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="AA119" s="7"/>
+      <c r="AB119" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC119" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="AD119" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE119" s="7"/>
+      <c r="AF119" s="7"/>
+      <c r="AG119" s="7"/>
+      <c r="AH119" s="7"/>
+      <c r="AI119" s="7"/>
+      <c r="AJ119" s="7"/>
+      <c r="AK119" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="120" spans="1:37">
+      <c r="A120" s="3">
+        <v>118</v>
+      </c>
+      <c r="B120" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C120" s="3">
+        <v>2025073567</v>
+      </c>
+      <c r="D120" s="3"/>
+      <c r="E120" s="3"/>
+      <c r="F120" s="3">
+        <v>4208</v>
+      </c>
+      <c r="G120" s="3" t="s">
+        <v>779</v>
+      </c>
+      <c r="H120" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="I120" s="3"/>
+      <c r="J120" s="3"/>
+      <c r="K120" s="3"/>
+      <c r="L120" s="3"/>
+      <c r="M120" s="4"/>
+      <c r="N120" s="3"/>
+      <c r="O120" s="4"/>
+      <c r="P120" s="10"/>
+      <c r="Q120" s="3" t="s">
+        <v>780</v>
+      </c>
+      <c r="R120" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S120" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="T120" s="3">
+        <v>1</v>
+      </c>
+      <c r="U120" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V120" s="3" t="s">
+        <v>781</v>
+      </c>
+      <c r="W120" s="3" t="s">
+        <v>782</v>
+      </c>
+      <c r="X120" s="3" t="s">
+        <v>783</v>
+      </c>
+      <c r="Y120" s="3"/>
+      <c r="Z120" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA120" s="3"/>
+      <c r="AB120" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC120" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="AD120" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE120" s="3"/>
+      <c r="AF120" s="3"/>
+      <c r="AG120" s="3"/>
+      <c r="AH120" s="3"/>
+      <c r="AI120" s="3"/>
+      <c r="AJ120" s="3"/>
+      <c r="AK120" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="121" spans="1:37">
+      <c r="A121" s="7">
+        <v>119</v>
+      </c>
+      <c r="B121" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C121" s="7">
+        <v>2025073568</v>
+      </c>
+      <c r="D121" s="7"/>
+      <c r="E121" s="7"/>
+      <c r="F121" s="7">
+        <v>4083</v>
+      </c>
+      <c r="G121" s="7" t="s">
+        <v>784</v>
+      </c>
+      <c r="H121" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I121" s="7"/>
+      <c r="J121" s="7"/>
+      <c r="K121" s="7"/>
+      <c r="L121" s="7"/>
+      <c r="M121" s="8"/>
+      <c r="N121" s="7"/>
+      <c r="O121" s="8"/>
+      <c r="P121" s="8"/>
+      <c r="Q121" s="7" t="s">
+        <v>785</v>
+      </c>
+      <c r="R121" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S121" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="T121" s="7">
+        <v>1</v>
+      </c>
+      <c r="U121" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V121" s="7" t="s">
+        <v>786</v>
+      </c>
+      <c r="W121" s="7" t="s">
+        <v>787</v>
+      </c>
+      <c r="X121" s="7" t="s">
+        <v>788</v>
+      </c>
+      <c r="Y121" s="7"/>
+      <c r="Z121" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="AA121" s="7"/>
+      <c r="AB121" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC121" s="8" t="s">
+        <v>355</v>
+      </c>
+      <c r="AD121" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE121" s="7"/>
+      <c r="AF121" s="7"/>
+      <c r="AG121" s="7"/>
+      <c r="AH121" s="7"/>
+      <c r="AI121" s="7"/>
+      <c r="AJ121" s="7"/>
+      <c r="AK121" s="7" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit on 29-2025-time
</commit_message>
<xml_diff>
--- a/IM/202507_HL_Maintain_Report.xlsx
+++ b/IM/202507_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$121</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$133</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="789">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202507   (  製表日期:2025-07-28  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="860">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202507   (  製表日期:2025-07-29  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -2357,6 +2357,36 @@
     <t>2025-07-28 11:26:00</t>
   </si>
   <si>
+    <t>14680114072801</t>
+  </si>
+  <si>
+    <t>板橋江寧店</t>
+  </si>
+  <si>
+    <t>2025-07-28 12:09:11</t>
+  </si>
+  <si>
+    <t>門市反應tm1 ccd掃描器(HC76-TR)未亮燈無電源反應...須請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF04680</t>
+  </si>
+  <si>
+    <t>2025-07-28 12:10:28</t>
+  </si>
+  <si>
+    <t>2025-07-29 14:10:00</t>
+  </si>
+  <si>
+    <t>2025-07-29 14:40:00</t>
+  </si>
+  <si>
+    <t>2025-07-29 16:10:00</t>
+  </si>
+  <si>
+    <t>重新接線後測試正常</t>
+  </si>
+  <si>
     <t>三重國隆店</t>
   </si>
   <si>
@@ -2445,6 +2475,195 @@
   </si>
   <si>
     <t>2025-07-28 15:03:00</t>
+  </si>
+  <si>
+    <t>15384114072801</t>
+  </si>
+  <si>
+    <t>2025-07-28 17:57:03</t>
+  </si>
+  <si>
+    <t>F603</t>
+  </si>
+  <si>
+    <t>門市反應TM1多卡機QP3000無法使用愛金卡，會顯示20C icasH卡片回應資料長度錯誤，客服已協助點選版更並點選手動開機授權仍顯示此訊息...請台芝到店協助</t>
+  </si>
+  <si>
+    <t>2025-07-28 17:58:01</t>
+  </si>
+  <si>
+    <t>2025-07-29 14:00:00</t>
+  </si>
+  <si>
+    <t>2025-07-29 15:32:00</t>
+  </si>
+  <si>
+    <t>2025-07-29 21:58:00</t>
+  </si>
+  <si>
+    <t>更換QP3000
+換上：8183003236
+換下：8183003587</t>
+  </si>
+  <si>
+    <t>15384114072802</t>
+  </si>
+  <si>
+    <t>2025-07-28 17:58:11</t>
+  </si>
+  <si>
+    <t>門市反應TM2多卡機QP3000無法使用愛金卡，會顯示20C icasH卡片回應資料長度錯誤，客服已協助點選版更並點選手動開機授權仍顯示此訊息...請台芝到店協助</t>
+  </si>
+  <si>
+    <t>2025-07-28 17:58:29</t>
+  </si>
+  <si>
+    <t>2025-07-29 15:35:00</t>
+  </si>
+  <si>
+    <t>更換QP3000
+換上：8183000474
+換下：8183003589</t>
+  </si>
+  <si>
+    <t>1L519114072801</t>
+  </si>
+  <si>
+    <t>L519</t>
+  </si>
+  <si>
+    <t>車麗屋林口店</t>
+  </si>
+  <si>
+    <t>2025-07-28 20:20:01</t>
+  </si>
+  <si>
+    <t>D302</t>
+  </si>
+  <si>
+    <t>發票印字不清</t>
+  </si>
+  <si>
+    <t>門市來電告知發票機(BSC-10)印字不清，已有將發票紙捲重放機器重開且有做基本清理仍無法排除，門市營業時間為10~21點，還請協助撥打電話聯繫.......還請台芝協助殷先生0922490547</t>
+  </si>
+  <si>
+    <t>THILF0L519</t>
+  </si>
+  <si>
+    <t>2025-07-28 20:22:33</t>
+  </si>
+  <si>
+    <t>2025-07-29 11:00:00</t>
+  </si>
+  <si>
+    <t>2025-07-29 12:00:00</t>
+  </si>
+  <si>
+    <t>2025-07-30 00:22:00</t>
+  </si>
+  <si>
+    <t>更換發票機
+換上8155006316
+換下8155003197</t>
+  </si>
+  <si>
+    <t>三重自強店</t>
+  </si>
+  <si>
+    <t>THILF03623</t>
+  </si>
+  <si>
+    <t>2025-07-29 12:07:22</t>
+  </si>
+  <si>
+    <t>2025-07-29 11:30:00</t>
+  </si>
+  <si>
+    <t>2025-07-29 12:21:39</t>
+  </si>
+  <si>
+    <t>2025-07-29 12:20:00</t>
+  </si>
+  <si>
+    <t>三重薔薇店</t>
+  </si>
+  <si>
+    <t>THILF04388</t>
+  </si>
+  <si>
+    <t>2025-07-29 13:20:11</t>
+  </si>
+  <si>
+    <t>2025-07-29 12:55:00</t>
+  </si>
+  <si>
+    <t>2025-07-29 13:18:00</t>
+  </si>
+  <si>
+    <t>D195</t>
+  </si>
+  <si>
+    <t>三重車路頭</t>
+  </si>
+  <si>
+    <t>THILF0D195</t>
+  </si>
+  <si>
+    <t>2025-07-29 13:55:08</t>
+  </si>
+  <si>
+    <t>2025-07-29 13:30:00</t>
+  </si>
+  <si>
+    <t>2025-07-29 13:54:00</t>
+  </si>
+  <si>
+    <t>三重商工店</t>
+  </si>
+  <si>
+    <t>THILF04652</t>
+  </si>
+  <si>
+    <t>2025-07-29 14:23:52</t>
+  </si>
+  <si>
+    <t>2025-07-29 14:23:00</t>
+  </si>
+  <si>
+    <t>2025-07-29 14:42:31</t>
+  </si>
+  <si>
+    <t>D390</t>
+  </si>
+  <si>
+    <t>三重大有店</t>
+  </si>
+  <si>
+    <t>THILF0D390</t>
+  </si>
+  <si>
+    <t>2025-07-29 15:27:22</t>
+  </si>
+  <si>
+    <t>2025-07-29 15:00:00</t>
+  </si>
+  <si>
+    <t>2025-07-29 15:26:00</t>
+  </si>
+  <si>
+    <t>三重穀保店</t>
+  </si>
+  <si>
+    <t>THILF04155</t>
+  </si>
+  <si>
+    <t>2025-07-29 15:55:04</t>
+  </si>
+  <si>
+    <t>2025-07-29 15:30:00</t>
+  </si>
+  <si>
+    <t>2025-07-29 15:54:00</t>
   </si>
 </sst>
 </file>
@@ -2858,10 +3077,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK121"/>
+  <dimension ref="A1:AK133"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A121" sqref="A121"/>
+      <selection activeCell="A133" sqref="A133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12499,38 +12718,58 @@
         <v>114</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>87</v>
+        <v>38</v>
       </c>
       <c r="C116" s="3">
-        <v>2025073542</v>
-      </c>
-      <c r="D116" s="3"/>
-      <c r="E116" s="3"/>
+        <v>2025073538</v>
+      </c>
+      <c r="D116" s="3" t="s">
+        <v>759</v>
+      </c>
+      <c r="E116" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="F116" s="3">
-        <v>4804</v>
+        <v>4680</v>
       </c>
       <c r="G116" s="3" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="H116" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="I116" s="3"/>
-      <c r="J116" s="3"/>
-      <c r="K116" s="3"/>
-      <c r="L116" s="3"/>
-      <c r="M116" s="4"/>
-      <c r="N116" s="3"/>
-      <c r="O116" s="4"/>
-      <c r="P116" s="10"/>
+        <v>64</v>
+      </c>
+      <c r="I116" s="3" t="s">
+        <v>761</v>
+      </c>
+      <c r="J116" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K116" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="L116" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="M116" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="N116" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="O116" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="P116" s="10" t="s">
+        <v>762</v>
+      </c>
       <c r="Q116" s="3" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
       <c r="R116" s="3" t="s">
         <v>52</v>
       </c>
       <c r="S116" s="3" t="s">
-        <v>53</v>
+        <v>74</v>
       </c>
       <c r="T116" s="3">
         <v>1</v>
@@ -12539,28 +12778,28 @@
         <v>54</v>
       </c>
       <c r="V116" s="3" t="s">
-        <v>761</v>
+        <v>764</v>
       </c>
       <c r="W116" s="3" t="s">
-        <v>762</v>
+        <v>765</v>
       </c>
       <c r="X116" s="3" t="s">
-        <v>763</v>
-      </c>
-      <c r="Y116" s="3"/>
+        <v>766</v>
+      </c>
+      <c r="Y116" s="3" t="s">
+        <v>767</v>
+      </c>
       <c r="Z116" s="3">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="AA116" s="3"/>
       <c r="AB116" s="3" t="s">
         <v>59</v>
       </c>
       <c r="AC116" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="AD116" s="3" t="s">
-        <v>61</v>
-      </c>
+        <v>768</v>
+      </c>
+      <c r="AD116" s="3"/>
       <c r="AE116" s="3"/>
       <c r="AF116" s="3"/>
       <c r="AG116" s="3"/>
@@ -12579,15 +12818,15 @@
         <v>87</v>
       </c>
       <c r="C117" s="7">
-        <v>2025073543</v>
+        <v>2025073542</v>
       </c>
       <c r="D117" s="7"/>
       <c r="E117" s="7"/>
       <c r="F117" s="7">
-        <v>4312</v>
+        <v>4804</v>
       </c>
       <c r="G117" s="7" t="s">
-        <v>764</v>
+        <v>769</v>
       </c>
       <c r="H117" s="7" t="s">
         <v>42</v>
@@ -12601,7 +12840,7 @@
       <c r="O117" s="8"/>
       <c r="P117" s="9"/>
       <c r="Q117" s="7" t="s">
-        <v>765</v>
+        <v>770</v>
       </c>
       <c r="R117" s="7" t="s">
         <v>52</v>
@@ -12616,17 +12855,17 @@
         <v>54</v>
       </c>
       <c r="V117" s="7" t="s">
-        <v>766</v>
+        <v>771</v>
       </c>
       <c r="W117" s="7" t="s">
-        <v>767</v>
+        <v>772</v>
       </c>
       <c r="X117" s="7" t="s">
-        <v>768</v>
+        <v>773</v>
       </c>
       <c r="Y117" s="7"/>
       <c r="Z117" s="7">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="AA117" s="7"/>
       <c r="AB117" s="7" t="s">
@@ -12656,15 +12895,15 @@
         <v>87</v>
       </c>
       <c r="C118" s="3">
-        <v>2025073544</v>
+        <v>2025073543</v>
       </c>
       <c r="D118" s="3"/>
       <c r="E118" s="3"/>
       <c r="F118" s="3">
-        <v>2619</v>
+        <v>4312</v>
       </c>
       <c r="G118" s="3" t="s">
-        <v>769</v>
+        <v>774</v>
       </c>
       <c r="H118" s="3" t="s">
         <v>42</v>
@@ -12678,7 +12917,7 @@
       <c r="O118" s="4"/>
       <c r="P118" s="10"/>
       <c r="Q118" s="3" t="s">
-        <v>770</v>
+        <v>775</v>
       </c>
       <c r="R118" s="3" t="s">
         <v>52</v>
@@ -12693,17 +12932,17 @@
         <v>54</v>
       </c>
       <c r="V118" s="3" t="s">
-        <v>771</v>
+        <v>776</v>
       </c>
       <c r="W118" s="3" t="s">
-        <v>772</v>
+        <v>777</v>
       </c>
       <c r="X118" s="3" t="s">
-        <v>773</v>
+        <v>778</v>
       </c>
       <c r="Y118" s="3"/>
       <c r="Z118" s="3">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="AA118" s="3"/>
       <c r="AB118" s="3" t="s">
@@ -12733,15 +12972,15 @@
         <v>87</v>
       </c>
       <c r="C119" s="7">
-        <v>2025073555</v>
+        <v>2025073544</v>
       </c>
       <c r="D119" s="7"/>
       <c r="E119" s="7"/>
       <c r="F119" s="7">
-        <v>2935</v>
+        <v>2619</v>
       </c>
       <c r="G119" s="7" t="s">
-        <v>774</v>
+        <v>779</v>
       </c>
       <c r="H119" s="7" t="s">
         <v>42</v>
@@ -12755,7 +12994,7 @@
       <c r="O119" s="8"/>
       <c r="P119" s="9"/>
       <c r="Q119" s="7" t="s">
-        <v>775</v>
+        <v>780</v>
       </c>
       <c r="R119" s="7" t="s">
         <v>52</v>
@@ -12770,17 +13009,17 @@
         <v>54</v>
       </c>
       <c r="V119" s="7" t="s">
-        <v>776</v>
+        <v>781</v>
       </c>
       <c r="W119" s="7" t="s">
-        <v>777</v>
+        <v>782</v>
       </c>
       <c r="X119" s="7" t="s">
-        <v>778</v>
+        <v>783</v>
       </c>
       <c r="Y119" s="7"/>
       <c r="Z119" s="7">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="AA119" s="7"/>
       <c r="AB119" s="7" t="s">
@@ -12810,18 +13049,18 @@
         <v>87</v>
       </c>
       <c r="C120" s="3">
-        <v>2025073567</v>
+        <v>2025073555</v>
       </c>
       <c r="D120" s="3"/>
       <c r="E120" s="3"/>
       <c r="F120" s="3">
-        <v>4208</v>
+        <v>2935</v>
       </c>
       <c r="G120" s="3" t="s">
-        <v>779</v>
+        <v>784</v>
       </c>
       <c r="H120" s="3" t="s">
-        <v>134</v>
+        <v>42</v>
       </c>
       <c r="I120" s="3"/>
       <c r="J120" s="3"/>
@@ -12832,13 +13071,13 @@
       <c r="O120" s="4"/>
       <c r="P120" s="10"/>
       <c r="Q120" s="3" t="s">
-        <v>780</v>
+        <v>785</v>
       </c>
       <c r="R120" s="3" t="s">
         <v>52</v>
       </c>
       <c r="S120" s="3" t="s">
-        <v>136</v>
+        <v>53</v>
       </c>
       <c r="T120" s="3">
         <v>1</v>
@@ -12847,17 +13086,17 @@
         <v>54</v>
       </c>
       <c r="V120" s="3" t="s">
-        <v>781</v>
+        <v>786</v>
       </c>
       <c r="W120" s="3" t="s">
-        <v>782</v>
+        <v>787</v>
       </c>
       <c r="X120" s="3" t="s">
-        <v>783</v>
+        <v>788</v>
       </c>
       <c r="Y120" s="3"/>
       <c r="Z120" s="3">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="AA120" s="3"/>
       <c r="AB120" s="3" t="s">
@@ -12887,18 +13126,18 @@
         <v>87</v>
       </c>
       <c r="C121" s="7">
-        <v>2025073568</v>
+        <v>2025073567</v>
       </c>
       <c r="D121" s="7"/>
       <c r="E121" s="7"/>
       <c r="F121" s="7">
-        <v>4083</v>
+        <v>4208</v>
       </c>
       <c r="G121" s="7" t="s">
-        <v>784</v>
+        <v>789</v>
       </c>
       <c r="H121" s="7" t="s">
-        <v>42</v>
+        <v>134</v>
       </c>
       <c r="I121" s="7"/>
       <c r="J121" s="7"/>
@@ -12907,15 +13146,15 @@
       <c r="M121" s="8"/>
       <c r="N121" s="7"/>
       <c r="O121" s="8"/>
-      <c r="P121" s="8"/>
+      <c r="P121" s="9"/>
       <c r="Q121" s="7" t="s">
-        <v>785</v>
+        <v>790</v>
       </c>
       <c r="R121" s="7" t="s">
         <v>52</v>
       </c>
       <c r="S121" s="7" t="s">
-        <v>53</v>
+        <v>136</v>
       </c>
       <c r="T121" s="7">
         <v>1</v>
@@ -12924,24 +13163,24 @@
         <v>54</v>
       </c>
       <c r="V121" s="7" t="s">
-        <v>786</v>
+        <v>791</v>
       </c>
       <c r="W121" s="7" t="s">
-        <v>787</v>
+        <v>792</v>
       </c>
       <c r="X121" s="7" t="s">
-        <v>788</v>
+        <v>793</v>
       </c>
       <c r="Y121" s="7"/>
       <c r="Z121" s="7">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="AA121" s="7"/>
       <c r="AB121" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="AC121" s="8" t="s">
-        <v>355</v>
+      <c r="AC121" s="9" t="s">
+        <v>95</v>
       </c>
       <c r="AD121" s="7" t="s">
         <v>61</v>
@@ -12953,6 +13192,990 @@
       <c r="AI121" s="7"/>
       <c r="AJ121" s="7"/>
       <c r="AK121" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="122" spans="1:37">
+      <c r="A122" s="3">
+        <v>120</v>
+      </c>
+      <c r="B122" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C122" s="3">
+        <v>2025073568</v>
+      </c>
+      <c r="D122" s="3"/>
+      <c r="E122" s="3"/>
+      <c r="F122" s="3">
+        <v>4083</v>
+      </c>
+      <c r="G122" s="3" t="s">
+        <v>794</v>
+      </c>
+      <c r="H122" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I122" s="3"/>
+      <c r="J122" s="3"/>
+      <c r="K122" s="3"/>
+      <c r="L122" s="3"/>
+      <c r="M122" s="4"/>
+      <c r="N122" s="3"/>
+      <c r="O122" s="4"/>
+      <c r="P122" s="10"/>
+      <c r="Q122" s="3" t="s">
+        <v>795</v>
+      </c>
+      <c r="R122" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S122" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T122" s="3">
+        <v>1</v>
+      </c>
+      <c r="U122" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V122" s="3" t="s">
+        <v>796</v>
+      </c>
+      <c r="W122" s="3" t="s">
+        <v>797</v>
+      </c>
+      <c r="X122" s="3" t="s">
+        <v>798</v>
+      </c>
+      <c r="Y122" s="3"/>
+      <c r="Z122" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="AA122" s="3"/>
+      <c r="AB122" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC122" s="10" t="s">
+        <v>355</v>
+      </c>
+      <c r="AD122" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE122" s="3"/>
+      <c r="AF122" s="3"/>
+      <c r="AG122" s="3"/>
+      <c r="AH122" s="3"/>
+      <c r="AI122" s="3"/>
+      <c r="AJ122" s="3"/>
+      <c r="AK122" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="123" spans="1:37">
+      <c r="A123" s="7">
+        <v>121</v>
+      </c>
+      <c r="B123" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C123" s="7">
+        <v>2025073625</v>
+      </c>
+      <c r="D123" s="7" t="s">
+        <v>799</v>
+      </c>
+      <c r="E123" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F123" s="7">
+        <v>5384</v>
+      </c>
+      <c r="G123" s="7" t="s">
+        <v>474</v>
+      </c>
+      <c r="H123" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="I123" s="7" t="s">
+        <v>800</v>
+      </c>
+      <c r="J123" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="K123" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="L123" s="7" t="s">
+        <v>566</v>
+      </c>
+      <c r="M123" s="8" t="s">
+        <v>567</v>
+      </c>
+      <c r="N123" s="7" t="s">
+        <v>801</v>
+      </c>
+      <c r="O123" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="P123" s="9" t="s">
+        <v>802</v>
+      </c>
+      <c r="Q123" s="7" t="s">
+        <v>475</v>
+      </c>
+      <c r="R123" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S123" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="T123" s="7">
+        <v>1</v>
+      </c>
+      <c r="U123" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V123" s="7" t="s">
+        <v>803</v>
+      </c>
+      <c r="W123" s="7" t="s">
+        <v>804</v>
+      </c>
+      <c r="X123" s="7" t="s">
+        <v>805</v>
+      </c>
+      <c r="Y123" s="7" t="s">
+        <v>806</v>
+      </c>
+      <c r="Z123" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="AA123" s="7"/>
+      <c r="AB123" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC123" s="9" t="s">
+        <v>807</v>
+      </c>
+      <c r="AD123" s="7"/>
+      <c r="AE123" s="7"/>
+      <c r="AF123" s="7"/>
+      <c r="AG123" s="7"/>
+      <c r="AH123" s="7"/>
+      <c r="AI123" s="7"/>
+      <c r="AJ123" s="7"/>
+      <c r="AK123" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="124" spans="1:37">
+      <c r="A124" s="3">
+        <v>122</v>
+      </c>
+      <c r="B124" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C124" s="3">
+        <v>2025073626</v>
+      </c>
+      <c r="D124" s="3" t="s">
+        <v>808</v>
+      </c>
+      <c r="E124" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F124" s="3">
+        <v>5384</v>
+      </c>
+      <c r="G124" s="3" t="s">
+        <v>474</v>
+      </c>
+      <c r="H124" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I124" s="3" t="s">
+        <v>809</v>
+      </c>
+      <c r="J124" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K124" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="L124" s="3" t="s">
+        <v>566</v>
+      </c>
+      <c r="M124" s="4" t="s">
+        <v>567</v>
+      </c>
+      <c r="N124" s="3" t="s">
+        <v>801</v>
+      </c>
+      <c r="O124" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="P124" s="10" t="s">
+        <v>810</v>
+      </c>
+      <c r="Q124" s="3" t="s">
+        <v>475</v>
+      </c>
+      <c r="R124" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S124" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="T124" s="3">
+        <v>1</v>
+      </c>
+      <c r="U124" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V124" s="3" t="s">
+        <v>811</v>
+      </c>
+      <c r="W124" s="3" t="s">
+        <v>804</v>
+      </c>
+      <c r="X124" s="3" t="s">
+        <v>812</v>
+      </c>
+      <c r="Y124" s="3" t="s">
+        <v>806</v>
+      </c>
+      <c r="Z124" s="3">
+        <v>1.6</v>
+      </c>
+      <c r="AA124" s="3"/>
+      <c r="AB124" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC124" s="10" t="s">
+        <v>813</v>
+      </c>
+      <c r="AD124" s="3"/>
+      <c r="AE124" s="3"/>
+      <c r="AF124" s="3"/>
+      <c r="AG124" s="3"/>
+      <c r="AH124" s="3"/>
+      <c r="AI124" s="3"/>
+      <c r="AJ124" s="3"/>
+      <c r="AK124" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="125" spans="1:37">
+      <c r="A125" s="7">
+        <v>123</v>
+      </c>
+      <c r="B125" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C125" s="7">
+        <v>2025073627</v>
+      </c>
+      <c r="D125" s="7" t="s">
+        <v>814</v>
+      </c>
+      <c r="E125" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F125" s="7" t="s">
+        <v>815</v>
+      </c>
+      <c r="G125" s="7" t="s">
+        <v>816</v>
+      </c>
+      <c r="H125" s="7" t="s">
+        <v>642</v>
+      </c>
+      <c r="I125" s="7" t="s">
+        <v>817</v>
+      </c>
+      <c r="J125" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="K125" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L125" s="7" t="s">
+        <v>544</v>
+      </c>
+      <c r="M125" s="8" t="s">
+        <v>545</v>
+      </c>
+      <c r="N125" s="7" t="s">
+        <v>818</v>
+      </c>
+      <c r="O125" s="8" t="s">
+        <v>819</v>
+      </c>
+      <c r="P125" s="9" t="s">
+        <v>820</v>
+      </c>
+      <c r="Q125" s="7" t="s">
+        <v>821</v>
+      </c>
+      <c r="R125" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S125" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="T125" s="7">
+        <v>1</v>
+      </c>
+      <c r="U125" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V125" s="7" t="s">
+        <v>822</v>
+      </c>
+      <c r="W125" s="7" t="s">
+        <v>823</v>
+      </c>
+      <c r="X125" s="7" t="s">
+        <v>824</v>
+      </c>
+      <c r="Y125" s="7" t="s">
+        <v>825</v>
+      </c>
+      <c r="Z125" s="7">
+        <v>1</v>
+      </c>
+      <c r="AA125" s="7"/>
+      <c r="AB125" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC125" s="9" t="s">
+        <v>826</v>
+      </c>
+      <c r="AD125" s="7"/>
+      <c r="AE125" s="7"/>
+      <c r="AF125" s="7"/>
+      <c r="AG125" s="7"/>
+      <c r="AH125" s="7"/>
+      <c r="AI125" s="7"/>
+      <c r="AJ125" s="7"/>
+      <c r="AK125" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="126" spans="1:37">
+      <c r="A126" s="3">
+        <v>124</v>
+      </c>
+      <c r="B126" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C126" s="3">
+        <v>2025073659</v>
+      </c>
+      <c r="D126" s="3"/>
+      <c r="E126" s="3"/>
+      <c r="F126" s="3">
+        <v>3623</v>
+      </c>
+      <c r="G126" s="3" t="s">
+        <v>827</v>
+      </c>
+      <c r="H126" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I126" s="3"/>
+      <c r="J126" s="3"/>
+      <c r="K126" s="3"/>
+      <c r="L126" s="3"/>
+      <c r="M126" s="4"/>
+      <c r="N126" s="3"/>
+      <c r="O126" s="4"/>
+      <c r="P126" s="10"/>
+      <c r="Q126" s="3" t="s">
+        <v>828</v>
+      </c>
+      <c r="R126" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S126" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T126" s="3">
+        <v>1</v>
+      </c>
+      <c r="U126" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V126" s="3" t="s">
+        <v>829</v>
+      </c>
+      <c r="W126" s="3" t="s">
+        <v>823</v>
+      </c>
+      <c r="X126" s="3" t="s">
+        <v>830</v>
+      </c>
+      <c r="Y126" s="3"/>
+      <c r="Z126" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA126" s="3"/>
+      <c r="AB126" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC126" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="AD126" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE126" s="3"/>
+      <c r="AF126" s="3"/>
+      <c r="AG126" s="3"/>
+      <c r="AH126" s="3"/>
+      <c r="AI126" s="3"/>
+      <c r="AJ126" s="3"/>
+      <c r="AK126" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="127" spans="1:37">
+      <c r="A127" s="7">
+        <v>125</v>
+      </c>
+      <c r="B127" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C127" s="7">
+        <v>2025073665</v>
+      </c>
+      <c r="D127" s="7"/>
+      <c r="E127" s="7"/>
+      <c r="F127" s="7" t="s">
+        <v>815</v>
+      </c>
+      <c r="G127" s="7" t="s">
+        <v>816</v>
+      </c>
+      <c r="H127" s="7" t="s">
+        <v>642</v>
+      </c>
+      <c r="I127" s="7"/>
+      <c r="J127" s="7"/>
+      <c r="K127" s="7"/>
+      <c r="L127" s="7"/>
+      <c r="M127" s="8"/>
+      <c r="N127" s="7"/>
+      <c r="O127" s="8"/>
+      <c r="P127" s="9"/>
+      <c r="Q127" s="7" t="s">
+        <v>821</v>
+      </c>
+      <c r="R127" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S127" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="T127" s="7">
+        <v>1</v>
+      </c>
+      <c r="U127" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V127" s="7" t="s">
+        <v>831</v>
+      </c>
+      <c r="W127" s="7" t="s">
+        <v>824</v>
+      </c>
+      <c r="X127" s="7" t="s">
+        <v>832</v>
+      </c>
+      <c r="Y127" s="7"/>
+      <c r="Z127" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA127" s="7"/>
+      <c r="AB127" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC127" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="AD127" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE127" s="7"/>
+      <c r="AF127" s="7"/>
+      <c r="AG127" s="7"/>
+      <c r="AH127" s="7"/>
+      <c r="AI127" s="7"/>
+      <c r="AJ127" s="7"/>
+      <c r="AK127" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="128" spans="1:37">
+      <c r="A128" s="3">
+        <v>126</v>
+      </c>
+      <c r="B128" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C128" s="3">
+        <v>2025073669</v>
+      </c>
+      <c r="D128" s="3"/>
+      <c r="E128" s="3"/>
+      <c r="F128" s="3">
+        <v>4388</v>
+      </c>
+      <c r="G128" s="3" t="s">
+        <v>833</v>
+      </c>
+      <c r="H128" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I128" s="3"/>
+      <c r="J128" s="3"/>
+      <c r="K128" s="3"/>
+      <c r="L128" s="3"/>
+      <c r="M128" s="4"/>
+      <c r="N128" s="3"/>
+      <c r="O128" s="4"/>
+      <c r="P128" s="10"/>
+      <c r="Q128" s="3" t="s">
+        <v>834</v>
+      </c>
+      <c r="R128" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S128" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T128" s="3">
+        <v>1</v>
+      </c>
+      <c r="U128" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V128" s="3" t="s">
+        <v>835</v>
+      </c>
+      <c r="W128" s="3" t="s">
+        <v>836</v>
+      </c>
+      <c r="X128" s="3" t="s">
+        <v>837</v>
+      </c>
+      <c r="Y128" s="3"/>
+      <c r="Z128" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="AA128" s="3"/>
+      <c r="AB128" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC128" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="AD128" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE128" s="3"/>
+      <c r="AF128" s="3"/>
+      <c r="AG128" s="3"/>
+      <c r="AH128" s="3"/>
+      <c r="AI128" s="3"/>
+      <c r="AJ128" s="3"/>
+      <c r="AK128" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="129" spans="1:37">
+      <c r="A129" s="7">
+        <v>127</v>
+      </c>
+      <c r="B129" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C129" s="7">
+        <v>2025073678</v>
+      </c>
+      <c r="D129" s="7"/>
+      <c r="E129" s="7"/>
+      <c r="F129" s="7" t="s">
+        <v>838</v>
+      </c>
+      <c r="G129" s="7" t="s">
+        <v>839</v>
+      </c>
+      <c r="H129" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I129" s="7"/>
+      <c r="J129" s="7"/>
+      <c r="K129" s="7"/>
+      <c r="L129" s="7"/>
+      <c r="M129" s="8"/>
+      <c r="N129" s="7"/>
+      <c r="O129" s="8"/>
+      <c r="P129" s="9"/>
+      <c r="Q129" s="7" t="s">
+        <v>840</v>
+      </c>
+      <c r="R129" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S129" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="T129" s="7">
+        <v>1</v>
+      </c>
+      <c r="U129" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V129" s="7" t="s">
+        <v>841</v>
+      </c>
+      <c r="W129" s="7" t="s">
+        <v>842</v>
+      </c>
+      <c r="X129" s="7" t="s">
+        <v>843</v>
+      </c>
+      <c r="Y129" s="7"/>
+      <c r="Z129" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="AA129" s="7"/>
+      <c r="AB129" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC129" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="AD129" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE129" s="7"/>
+      <c r="AF129" s="7"/>
+      <c r="AG129" s="7"/>
+      <c r="AH129" s="7"/>
+      <c r="AI129" s="7"/>
+      <c r="AJ129" s="7"/>
+      <c r="AK129" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="130" spans="1:37">
+      <c r="A130" s="3">
+        <v>128</v>
+      </c>
+      <c r="B130" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C130" s="3">
+        <v>2025073684</v>
+      </c>
+      <c r="D130" s="3"/>
+      <c r="E130" s="3"/>
+      <c r="F130" s="3">
+        <v>4652</v>
+      </c>
+      <c r="G130" s="3" t="s">
+        <v>844</v>
+      </c>
+      <c r="H130" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I130" s="3"/>
+      <c r="J130" s="3"/>
+      <c r="K130" s="3"/>
+      <c r="L130" s="3"/>
+      <c r="M130" s="4"/>
+      <c r="N130" s="3"/>
+      <c r="O130" s="4"/>
+      <c r="P130" s="10"/>
+      <c r="Q130" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="R130" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S130" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T130" s="3">
+        <v>1</v>
+      </c>
+      <c r="U130" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V130" s="3" t="s">
+        <v>846</v>
+      </c>
+      <c r="W130" s="3" t="s">
+        <v>804</v>
+      </c>
+      <c r="X130" s="3" t="s">
+        <v>847</v>
+      </c>
+      <c r="Y130" s="3"/>
+      <c r="Z130" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="AA130" s="3"/>
+      <c r="AB130" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC130" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="AD130" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE130" s="3"/>
+      <c r="AF130" s="3"/>
+      <c r="AG130" s="3"/>
+      <c r="AH130" s="3"/>
+      <c r="AI130" s="3"/>
+      <c r="AJ130" s="3"/>
+      <c r="AK130" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="131" spans="1:37">
+      <c r="A131" s="7">
+        <v>129</v>
+      </c>
+      <c r="B131" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C131" s="7">
+        <v>2025073687</v>
+      </c>
+      <c r="D131" s="7"/>
+      <c r="E131" s="7"/>
+      <c r="F131" s="7">
+        <v>4680</v>
+      </c>
+      <c r="G131" s="7" t="s">
+        <v>760</v>
+      </c>
+      <c r="H131" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="I131" s="7"/>
+      <c r="J131" s="7"/>
+      <c r="K131" s="7"/>
+      <c r="L131" s="7"/>
+      <c r="M131" s="8"/>
+      <c r="N131" s="7"/>
+      <c r="O131" s="8"/>
+      <c r="P131" s="9"/>
+      <c r="Q131" s="7" t="s">
+        <v>763</v>
+      </c>
+      <c r="R131" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S131" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="T131" s="7">
+        <v>1</v>
+      </c>
+      <c r="U131" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V131" s="7" t="s">
+        <v>848</v>
+      </c>
+      <c r="W131" s="7" t="s">
+        <v>765</v>
+      </c>
+      <c r="X131" s="7" t="s">
+        <v>766</v>
+      </c>
+      <c r="Y131" s="7"/>
+      <c r="Z131" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA131" s="7"/>
+      <c r="AB131" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC131" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="AD131" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE131" s="7"/>
+      <c r="AF131" s="7"/>
+      <c r="AG131" s="7"/>
+      <c r="AH131" s="7"/>
+      <c r="AI131" s="7"/>
+      <c r="AJ131" s="7"/>
+      <c r="AK131" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="132" spans="1:37">
+      <c r="A132" s="3">
+        <v>130</v>
+      </c>
+      <c r="B132" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C132" s="3">
+        <v>2025073696</v>
+      </c>
+      <c r="D132" s="3"/>
+      <c r="E132" s="3"/>
+      <c r="F132" s="3" t="s">
+        <v>849</v>
+      </c>
+      <c r="G132" s="3" t="s">
+        <v>850</v>
+      </c>
+      <c r="H132" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I132" s="3"/>
+      <c r="J132" s="3"/>
+      <c r="K132" s="3"/>
+      <c r="L132" s="3"/>
+      <c r="M132" s="4"/>
+      <c r="N132" s="3"/>
+      <c r="O132" s="4"/>
+      <c r="P132" s="10"/>
+      <c r="Q132" s="3" t="s">
+        <v>851</v>
+      </c>
+      <c r="R132" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S132" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T132" s="3">
+        <v>1</v>
+      </c>
+      <c r="U132" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V132" s="3" t="s">
+        <v>852</v>
+      </c>
+      <c r="W132" s="3" t="s">
+        <v>853</v>
+      </c>
+      <c r="X132" s="3" t="s">
+        <v>854</v>
+      </c>
+      <c r="Y132" s="3"/>
+      <c r="Z132" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="AA132" s="3"/>
+      <c r="AB132" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC132" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="AD132" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE132" s="3"/>
+      <c r="AF132" s="3"/>
+      <c r="AG132" s="3"/>
+      <c r="AH132" s="3"/>
+      <c r="AI132" s="3"/>
+      <c r="AJ132" s="3"/>
+      <c r="AK132" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="133" spans="1:37">
+      <c r="A133" s="7">
+        <v>131</v>
+      </c>
+      <c r="B133" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C133" s="7">
+        <v>2025073701</v>
+      </c>
+      <c r="D133" s="7"/>
+      <c r="E133" s="7"/>
+      <c r="F133" s="7">
+        <v>4155</v>
+      </c>
+      <c r="G133" s="7" t="s">
+        <v>855</v>
+      </c>
+      <c r="H133" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I133" s="7"/>
+      <c r="J133" s="7"/>
+      <c r="K133" s="7"/>
+      <c r="L133" s="7"/>
+      <c r="M133" s="8"/>
+      <c r="N133" s="7"/>
+      <c r="O133" s="8"/>
+      <c r="P133" s="8"/>
+      <c r="Q133" s="7" t="s">
+        <v>856</v>
+      </c>
+      <c r="R133" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S133" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="T133" s="7">
+        <v>1</v>
+      </c>
+      <c r="U133" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V133" s="7" t="s">
+        <v>857</v>
+      </c>
+      <c r="W133" s="7" t="s">
+        <v>858</v>
+      </c>
+      <c r="X133" s="7" t="s">
+        <v>859</v>
+      </c>
+      <c r="Y133" s="7"/>
+      <c r="Z133" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="AA133" s="7"/>
+      <c r="AB133" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC133" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="AD133" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE133" s="7"/>
+      <c r="AF133" s="7"/>
+      <c r="AG133" s="7"/>
+      <c r="AH133" s="7"/>
+      <c r="AI133" s="7"/>
+      <c r="AJ133" s="7"/>
+      <c r="AK133" s="7" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 08041709
</commit_message>
<xml_diff>
--- a/IM/202507_HL_Maintain_Report.xlsx
+++ b/IM/202507_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$133</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$134</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="860">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202507   (  製表日期:2025-07-30  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="874">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202507   (  製表日期:2025-08-04  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -2664,6 +2664,49 @@
   </si>
   <si>
     <t>2025-07-29 15:54:00</t>
+  </si>
+  <si>
+    <t>1T100114073001</t>
+  </si>
+  <si>
+    <t>T100</t>
+  </si>
+  <si>
+    <t>五股訓練教室027401</t>
+  </si>
+  <si>
+    <t>2025-07-30 13:56:54</t>
+  </si>
+  <si>
+    <t>HL24</t>
+  </si>
+  <si>
+    <t>HL-SC主機</t>
+  </si>
+  <si>
+    <t>當機/自動開關機</t>
+  </si>
+  <si>
+    <t>楊小姐反應T100訓練教室雷射印表機(EPL6200)頻繁發生無法使用異狀，需請台芝到店協助確認異常 PS.地址:新北市五股區五工六路28號2樓
+聯絡人:0935114452楊小姐</t>
+  </si>
+  <si>
+    <t>THILF0T100</t>
+  </si>
+  <si>
+    <t>2025-07-30 14:12:09</t>
+  </si>
+  <si>
+    <t>2025-07-31 14:00:00</t>
+  </si>
+  <si>
+    <t>2025-07-31 15:30:00</t>
+  </si>
+  <si>
+    <t>2025-07-31 18:12:00</t>
+  </si>
+  <si>
+    <t>現場測試正常  無法列印已排除</t>
   </si>
 </sst>
 </file>
@@ -3077,10 +3120,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK133"/>
+  <dimension ref="A1:AK134"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A133" sqref="A133"/>
+      <selection activeCell="AC131" sqref="AC131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14130,7 +14173,7 @@
       <c r="M133" s="8"/>
       <c r="N133" s="7"/>
       <c r="O133" s="8"/>
-      <c r="P133" s="8"/>
+      <c r="P133" s="9"/>
       <c r="Q133" s="7" t="s">
         <v>856</v>
       </c>
@@ -14163,7 +14206,7 @@
       <c r="AB133" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="AC133" s="8" t="s">
+      <c r="AC133" s="9" t="s">
         <v>95</v>
       </c>
       <c r="AD133" s="7" t="s">
@@ -14176,6 +14219,103 @@
       <c r="AI133" s="7"/>
       <c r="AJ133" s="7"/>
       <c r="AK133" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="134" spans="1:37">
+      <c r="A134" s="3">
+        <v>132</v>
+      </c>
+      <c r="B134" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C134" s="3">
+        <v>2025073768</v>
+      </c>
+      <c r="D134" s="3" t="s">
+        <v>860</v>
+      </c>
+      <c r="E134" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F134" s="3" t="s">
+        <v>861</v>
+      </c>
+      <c r="G134" s="3" t="s">
+        <v>862</v>
+      </c>
+      <c r="H134" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="I134" s="3" t="s">
+        <v>863</v>
+      </c>
+      <c r="J134" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="K134" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="L134" s="3" t="s">
+        <v>864</v>
+      </c>
+      <c r="M134" s="4" t="s">
+        <v>865</v>
+      </c>
+      <c r="N134" s="3">
+        <v>2401</v>
+      </c>
+      <c r="O134" s="4" t="s">
+        <v>866</v>
+      </c>
+      <c r="P134" s="4" t="s">
+        <v>867</v>
+      </c>
+      <c r="Q134" s="3" t="s">
+        <v>868</v>
+      </c>
+      <c r="R134" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S134" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="T134" s="3">
+        <v>1</v>
+      </c>
+      <c r="U134" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V134" s="3" t="s">
+        <v>869</v>
+      </c>
+      <c r="W134" s="3" t="s">
+        <v>870</v>
+      </c>
+      <c r="X134" s="3" t="s">
+        <v>871</v>
+      </c>
+      <c r="Y134" s="3" t="s">
+        <v>872</v>
+      </c>
+      <c r="Z134" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="AA134" s="3"/>
+      <c r="AB134" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC134" s="4" t="s">
+        <v>873</v>
+      </c>
+      <c r="AD134" s="3"/>
+      <c r="AE134" s="3"/>
+      <c r="AF134" s="3"/>
+      <c r="AG134" s="3"/>
+      <c r="AH134" s="3"/>
+      <c r="AI134" s="3"/>
+      <c r="AJ134" s="3"/>
+      <c r="AK134" s="3" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>